<commit_message>
Got more time. Savepoint before weighted means
</commit_message>
<xml_diff>
--- a/monsoon/Calculations/Testing Numbers.xlsx
+++ b/monsoon/Calculations/Testing Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinimlay/Documents/School/graduate/CS685 - Graduate Research/kmeans_mpi/monsoon/Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3B5AD4-74BA-2E4C-A63B-E3608C695F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F01EFF-59EE-164F-986E-31C10B7E8CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="6" xr2:uid="{BC4CF94B-A0A3-6D4F-B231-01F23389F441}"/>
   </bookViews>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="14">
   <si>
     <t>MSD</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>MPI Yinyang</t>
+  </si>
+  <si>
+    <t>MPI+OMP Yinyang</t>
+  </si>
+  <si>
+    <t>MPI+OMP Lloyd</t>
   </si>
 </sst>
 </file>
@@ -1520,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24136027-FD2B-284F-ADEB-07FF9A49C47B}">
   <dimension ref="A1:G160"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3439,7 +3445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B682A04A-CC85-1940-9E8B-CB14A8C8A0B3}">
   <dimension ref="A1:G160"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
@@ -5356,34 +5362,2231 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EBC1F6-D14E-FF47-8259-74512AC8FF74}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A71" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77:D102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>0.3266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0.60170000000000001</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0.4758</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0.32869999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>0.48680000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0.50539999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>0.52980000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0.48139999999999999</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>128</v>
+      </c>
+      <c r="D12">
+        <v>1.4481999999999999</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>1.2653000000000001</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>1.2279</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <v>1.2217</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>1.2694000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>512</v>
+      </c>
+      <c r="D17">
+        <v>4.6298000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1">
+        <v>4.2732000000000001</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
+        <v>7.56</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <v>4.2864000000000004</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <v>4.2614000000000001</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>1024</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <v>8.3788</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <v>8.3972999999999995</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+      <c r="D24">
+        <v>8.3735999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>8.3584999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <v>8.3810000000000002</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>0.41099999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0.40279999999999999</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>0.4022</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>0.40679999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <v>0.57010000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>1.0147999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>0.59789999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>0.66149999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>0.59560000000000002</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>128</v>
+      </c>
+      <c r="D37">
+        <v>1.2344999999999999</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>1.2650999999999999</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>1.3124</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <v>1.3525</v>
+      </c>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>1.3562000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>512</v>
+      </c>
+      <c r="D42">
+        <v>3.6631</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1">
+        <v>3.6878000000000002</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+      <c r="D44" s="1">
+        <v>3.6126999999999998</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1">
+        <v>3.9582000000000002</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1">
+        <v>3.6806000000000001</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>1024</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1">
+        <v>6.7306999999999997</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C48" s="1"/>
+      <c r="D48" s="1">
+        <v>6.702</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C49" s="1"/>
+      <c r="D49">
+        <v>6.7062999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <v>7.4964000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1">
+        <v>6.9032999999999998</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>8</v>
+      </c>
+      <c r="D52">
+        <v>0.56589999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>0.42809999999999998</v>
+      </c>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <v>0.34320000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <v>0.48730000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>0.3952</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>32</v>
+      </c>
+      <c r="D57">
+        <v>0.54890000000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>0.2437</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <v>0.64429999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <v>0.40899999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>0.55120000000000002</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>128</v>
+      </c>
+      <c r="D62">
+        <v>0.33079999999999998</v>
+      </c>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <v>0.61819999999999997</v>
+      </c>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <v>0.44969999999999999</v>
+      </c>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D65" s="2">
+        <v>0.35920000000000002</v>
+      </c>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <v>0.82799999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>512</v>
+      </c>
+      <c r="D67">
+        <v>1.1168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1">
+        <v>1.0091000000000001</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1">
+        <v>1.0227999999999999</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C70" s="1"/>
+      <c r="D70" s="1">
+        <v>1.3541000000000001</v>
+      </c>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C71" s="1"/>
+      <c r="D71" s="1">
+        <v>1.0356000000000001</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>1024</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1">
+        <v>1.8874</v>
+      </c>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C73" s="1"/>
+      <c r="D73" s="1">
+        <v>2.1486000000000001</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C74" s="1"/>
+      <c r="D74">
+        <v>2.0699000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <v>2.2624</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C76" s="1"/>
+      <c r="D76" s="1">
+        <v>1.7638</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>32</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="D77">
+        <v>0.3523</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>0.61329999999999996</v>
+      </c>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <v>0.43919999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <v>0.73199999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <v>0.57830000000000004</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>32</v>
+      </c>
+      <c r="D82">
+        <v>0.50270000000000004</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <v>0.66879999999999995</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>0.55989999999999995</v>
+      </c>
+      <c r="E86" s="2"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>128</v>
+      </c>
+      <c r="D87">
+        <v>0.2702</v>
+      </c>
+      <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <v>0.75539999999999996</v>
+      </c>
+      <c r="F89" s="1"/>
+    </row>
+    <row r="90" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="D90" s="2">
+        <v>0.53390000000000004</v>
+      </c>
+      <c r="F90" s="1"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>512</v>
+      </c>
+      <c r="D92">
+        <v>0.60289999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C93" s="1"/>
+      <c r="D93" s="1">
+        <v>0.70309999999999995</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+    </row>
+    <row r="94" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C94" s="1"/>
+      <c r="D94" s="1">
+        <v>0.8972</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C95" s="1"/>
+      <c r="D95" s="1">
+        <v>0.79110000000000003</v>
+      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C96" s="1"/>
+      <c r="D96" s="1">
+        <v>0.94320000000000004</v>
+      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>1024</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1">
+        <v>1.2408999999999999</v>
+      </c>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+    </row>
+    <row r="98" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
+      <c r="D98" s="1">
+        <v>1.0250999999999999</v>
+      </c>
+      <c r="E98" s="2"/>
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C99" s="1"/>
+      <c r="D99">
+        <v>1.3651</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <v>1.4689000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C101" s="1"/>
+      <c r="D101" s="1">
+        <v>1.2009000000000001</v>
+      </c>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D34EA2-A2C1-4543-B890-D5580BFD39EC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>0.59609999999999996</v>
+      </c>
+      <c r="D2">
+        <v>1.6489</v>
+      </c>
+      <c r="E2">
+        <v>1.5894999999999999</v>
+      </c>
+      <c r="F2">
+        <v>5.5754999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.60540000000000005</v>
+      </c>
+      <c r="D3">
+        <v>1.6463000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.4662999999999999</v>
+      </c>
+      <c r="F3">
+        <v>6.2497999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0.59540000000000004</v>
+      </c>
+      <c r="D4">
+        <v>1.6752</v>
+      </c>
+      <c r="E4">
+        <v>1.6311</v>
+      </c>
+      <c r="F4">
+        <v>5.7502000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>0.59519999999999995</v>
+      </c>
+      <c r="D5">
+        <v>1.7267999999999999</v>
+      </c>
+      <c r="E5">
+        <v>1.5452999999999999</v>
+      </c>
+      <c r="F5">
+        <v>5.3121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>0.59609999999999996</v>
+      </c>
+      <c r="D6">
+        <v>5.8902999999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.5774999999999999</v>
+      </c>
+      <c r="F6">
+        <v>4.9172000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>1.8079000000000001</v>
+      </c>
+      <c r="D7">
+        <v>5.3921999999999999</v>
+      </c>
+      <c r="E7">
+        <v>4.2415000000000003</v>
+      </c>
+      <c r="F7">
+        <v>12.1296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1.8047</v>
+      </c>
+      <c r="D8">
+        <v>5.3593999999999999</v>
+      </c>
+      <c r="E8">
+        <v>4.1932999999999998</v>
+      </c>
+      <c r="F8">
+        <v>12.5039</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>1.8053999999999999</v>
+      </c>
+      <c r="D9">
+        <v>5.3818000000000001</v>
+      </c>
+      <c r="E9">
+        <v>4.4850000000000003</v>
+      </c>
+      <c r="F9">
+        <v>12.626300000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1.8064</v>
+      </c>
+      <c r="D10">
+        <v>5.3513999999999999</v>
+      </c>
+      <c r="E10">
+        <v>4.2774999999999999</v>
+      </c>
+      <c r="F10">
+        <v>12.0265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1.8029999999999999</v>
+      </c>
+      <c r="D11">
+        <v>20.022200000000002</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.6241000000000003</v>
+      </c>
+      <c r="F11" s="1">
+        <v>12.104200000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>128</v>
+      </c>
+      <c r="C12">
+        <v>6.1776999999999997</v>
+      </c>
+      <c r="D12">
+        <v>20.160499999999999</v>
+      </c>
+      <c r="E12">
+        <v>14.8102</v>
+      </c>
+      <c r="F12" s="1">
+        <v>42.821199999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>6.1806000000000001</v>
+      </c>
+      <c r="D13">
+        <v>20.0212</v>
+      </c>
+      <c r="E13">
+        <v>14.4849</v>
+      </c>
+      <c r="F13" s="1">
+        <v>43.080399999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>6.1882999999999999</v>
+      </c>
+      <c r="D14">
+        <v>20.054200000000002</v>
+      </c>
+      <c r="E14">
+        <v>14.253399999999999</v>
+      </c>
+      <c r="F14" s="1">
+        <v>43.089799999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>6.1658999999999997</v>
+      </c>
+      <c r="D15" s="2">
+        <v>20.376899999999999</v>
+      </c>
+      <c r="E15">
+        <v>14.447699999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>42.850099999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>6.1917</v>
+      </c>
+      <c r="D16">
+        <v>78.286000000000001</v>
+      </c>
+      <c r="E16">
+        <v>14.4467</v>
+      </c>
+      <c r="F16">
+        <v>42.822600000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>512</v>
+      </c>
+      <c r="C17">
+        <v>23.415600000000001</v>
+      </c>
+      <c r="D17">
+        <v>77.997200000000007</v>
+      </c>
+      <c r="E17">
+        <v>52.051499999999997</v>
+      </c>
+      <c r="F17">
+        <v>61.628399999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="1">
+        <v>23.371600000000001</v>
+      </c>
+      <c r="D18" s="1">
+        <v>77.992099999999994</v>
+      </c>
+      <c r="E18" s="1">
+        <v>52.097299999999997</v>
+      </c>
+      <c r="F18" s="1">
+        <v>161.91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>23.436199999999999</v>
+      </c>
+      <c r="D19" s="1">
+        <v>77.7346</v>
+      </c>
+      <c r="E19" s="2">
+        <v>52.618000000000002</v>
+      </c>
+      <c r="F19" s="1">
+        <v>162.11879999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="1">
+        <v>23.396899999999999</v>
+      </c>
+      <c r="D20" s="1">
+        <v>77.825299999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <v>52.580800000000004</v>
+      </c>
+      <c r="F20" s="1">
+        <v>162.0188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="1">
+        <v>23.438300000000002</v>
+      </c>
+      <c r="D21" s="1">
+        <v>155.10429999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>52.238500000000002</v>
+      </c>
+      <c r="F21" s="1">
+        <v>162.06229999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>1024</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44.732500000000002</v>
+      </c>
+      <c r="D22" s="1">
+        <v>154.9546</v>
+      </c>
+      <c r="E22" s="1">
+        <v>103.1284</v>
+      </c>
+      <c r="F22" s="1">
+        <v>319.23719999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>44.721699999999998</v>
+      </c>
+      <c r="D23" s="1">
+        <v>154.99719999999999</v>
+      </c>
+      <c r="E23" s="2">
+        <v>103.04170000000001</v>
+      </c>
+      <c r="F23" s="1">
+        <v>318.06310000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="1">
+        <v>44.610500000000002</v>
+      </c>
+      <c r="D24">
+        <v>154.86320000000001</v>
+      </c>
+      <c r="E24">
+        <v>102.9044</v>
+      </c>
+      <c r="F24">
+        <v>319.0883</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>44.702199999999998</v>
+      </c>
+      <c r="D25">
+        <v>155.10579999999999</v>
+      </c>
+      <c r="E25">
+        <v>102.87609999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="1">
+        <v>44.674900000000001</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1">
+        <v>102.84990000000001</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>1.5396000000000001</v>
+      </c>
+      <c r="D27">
+        <v>1.6937</v>
+      </c>
+      <c r="E27">
+        <v>1.4732000000000001</v>
+      </c>
+      <c r="F27">
+        <v>5.0118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1.4228000000000001</v>
+      </c>
+      <c r="D28">
+        <v>1.7022999999999999</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.2991999999999999</v>
+      </c>
+      <c r="F28">
+        <v>5.1195000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>1.5432999999999999</v>
+      </c>
+      <c r="D29">
+        <v>1.6589</v>
+      </c>
+      <c r="E29">
+        <v>1.6939</v>
+      </c>
+      <c r="F29">
+        <v>5.141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>1.9629000000000001</v>
+      </c>
+      <c r="D30">
+        <v>1.7081</v>
+      </c>
+      <c r="E30">
+        <v>1.3066</v>
+      </c>
+      <c r="F30">
+        <v>4.5923999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>1.4745999999999999</v>
+      </c>
+      <c r="D31">
+        <v>1.6496999999999999</v>
+      </c>
+      <c r="E31">
+        <v>1.4347000000000001</v>
+      </c>
+      <c r="F31">
+        <v>9.3696999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>32</v>
+      </c>
+      <c r="C32">
+        <v>3.4657</v>
+      </c>
+      <c r="D32">
+        <v>5.2729999999999997</v>
+      </c>
+      <c r="E32">
+        <v>3.7852999999999999</v>
+      </c>
+      <c r="F32">
+        <v>11.7766</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>3.9815</v>
+      </c>
+      <c r="D33">
+        <v>5.2731000000000003</v>
+      </c>
+      <c r="E33">
+        <v>3.7957000000000001</v>
+      </c>
+      <c r="F33">
+        <v>12.238899999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>2.5756000000000001</v>
+      </c>
+      <c r="D34">
+        <v>5.5362</v>
+      </c>
+      <c r="E34">
+        <v>3.9695999999999998</v>
+      </c>
+      <c r="F34">
+        <v>11.824</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>1.9407000000000001</v>
+      </c>
+      <c r="D35">
+        <v>5.4512999999999998</v>
+      </c>
+      <c r="E35">
+        <v>3.8567999999999998</v>
+      </c>
+      <c r="F35">
+        <v>11.951700000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>2.6661999999999999</v>
+      </c>
+      <c r="D36">
+        <v>5.4019000000000004</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3.8188</v>
+      </c>
+      <c r="F36" s="1">
+        <v>11.9009</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>128</v>
+      </c>
+      <c r="C37">
+        <v>7.4875999999999996</v>
+      </c>
+      <c r="D37">
+        <v>20.225200000000001</v>
+      </c>
+      <c r="E37">
+        <v>13.7829</v>
+      </c>
+      <c r="F37" s="1">
+        <v>43.038899999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>8.0985999999999994</v>
+      </c>
+      <c r="D38">
+        <v>19.958200000000001</v>
+      </c>
+      <c r="E38">
+        <v>13.575699999999999</v>
+      </c>
+      <c r="F38" s="1">
+        <v>43.519399999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>7.9722999999999997</v>
+      </c>
+      <c r="D39">
+        <v>20.169</v>
+      </c>
+      <c r="E39">
+        <v>13.4579</v>
+      </c>
+      <c r="F39" s="1">
+        <v>43.104100000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>7.7778999999999998</v>
+      </c>
+      <c r="D40" s="2">
+        <v>21.2654</v>
+      </c>
+      <c r="E40">
+        <v>13.7514</v>
+      </c>
+      <c r="F40" s="1">
+        <v>43.308900000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>8.2012</v>
+      </c>
+      <c r="D41">
+        <v>19.924399999999999</v>
+      </c>
+      <c r="E41">
+        <v>13.6228</v>
+      </c>
+      <c r="F41">
+        <v>46.264099999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>512</v>
+      </c>
+      <c r="C42">
+        <v>25.2241</v>
+      </c>
+      <c r="D42">
+        <v>77.8339</v>
+      </c>
+      <c r="E42">
+        <v>49.962899999999998</v>
+      </c>
+      <c r="F42">
+        <v>162.7482</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C43" s="1">
+        <v>26.2592</v>
+      </c>
+      <c r="D43" s="1">
+        <v>77.778199999999998</v>
+      </c>
+      <c r="E43" s="1">
+        <v>50.1554</v>
+      </c>
+      <c r="F43" s="1">
+        <v>161.935</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C44" s="1">
+        <v>25.227799999999998</v>
+      </c>
+      <c r="D44" s="1">
+        <v>77.674700000000001</v>
+      </c>
+      <c r="E44" s="2">
+        <v>49.886800000000001</v>
+      </c>
+      <c r="F44" s="1">
+        <v>162.24639999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C45" s="1">
+        <v>26.371099999999998</v>
+      </c>
+      <c r="D45" s="1">
+        <v>77.619900000000001</v>
+      </c>
+      <c r="E45" s="1">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="F45" s="1">
+        <v>163.25489999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C46" s="1">
+        <v>26.3522</v>
+      </c>
+      <c r="D46" s="1">
+        <v>77.929000000000002</v>
+      </c>
+      <c r="E46" s="1">
+        <v>49.900799999999997</v>
+      </c>
+      <c r="F46" s="1">
+        <v>162.29920000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>1024</v>
+      </c>
+      <c r="C47" s="1">
+        <v>47.673000000000002</v>
+      </c>
+      <c r="D47" s="1">
+        <v>154.9135</v>
+      </c>
+      <c r="E47" s="1">
+        <v>98.203000000000003</v>
+      </c>
+      <c r="F47" s="1">
+        <v>319.76889999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <v>47.556399999999996</v>
+      </c>
+      <c r="D48" s="1">
+        <v>155.0735</v>
+      </c>
+      <c r="E48" s="2">
+        <v>98.234099999999998</v>
+      </c>
+      <c r="F48" s="1">
+        <v>319.161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C49" s="1">
+        <v>48.134900000000002</v>
+      </c>
+      <c r="D49">
+        <v>155.0334</v>
+      </c>
+      <c r="E49">
+        <v>98.367800000000003</v>
+      </c>
+      <c r="F49">
+        <v>320.36439999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>47.903700000000001</v>
+      </c>
+      <c r="D50">
+        <v>155.10409999999999</v>
+      </c>
+      <c r="E50">
+        <v>98.306899999999999</v>
+      </c>
+      <c r="F50">
+        <v>318.32990000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="1">
+        <v>47.841500000000003</v>
+      </c>
+      <c r="D51" s="1">
+        <v>155.11250000000001</v>
+      </c>
+      <c r="E51" s="1">
+        <v>98.613</v>
+      </c>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>0.79</v>
+      </c>
+      <c r="D52">
+        <v>1.8668</v>
+      </c>
+      <c r="E52">
+        <v>1.3684000000000001</v>
+      </c>
+      <c r="F52">
+        <v>4.2038000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>0.66569999999999996</v>
+      </c>
+      <c r="D53">
+        <v>1.7611000000000001</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1.2955000000000001</v>
+      </c>
+      <c r="F53">
+        <v>4.2023999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>0.7147</v>
+      </c>
+      <c r="D54">
+        <v>1.9019999999999999</v>
+      </c>
+      <c r="E54">
+        <v>1.3983000000000001</v>
+      </c>
+      <c r="F54">
+        <v>4.3909000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="D55">
+        <v>1.7049000000000001</v>
+      </c>
+      <c r="E55">
+        <v>1.393</v>
+      </c>
+      <c r="F55">
+        <v>4.4523999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>0.73260000000000003</v>
+      </c>
+      <c r="D56">
+        <v>1.6954</v>
+      </c>
+      <c r="E56">
+        <v>1.3187</v>
+      </c>
+      <c r="F56">
+        <v>5.1688999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>32</v>
+      </c>
+      <c r="C57">
+        <v>1.9790000000000001</v>
+      </c>
+      <c r="D57">
+        <v>5.4588999999999999</v>
+      </c>
+      <c r="E57">
+        <v>3.8170000000000002</v>
+      </c>
+      <c r="F57">
+        <v>11.171200000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <v>1.9842</v>
+      </c>
+      <c r="D58">
+        <v>5.4718999999999998</v>
+      </c>
+      <c r="E58">
+        <v>3.9439000000000002</v>
+      </c>
+      <c r="F58">
+        <v>10.544499999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <v>2.0844</v>
+      </c>
+      <c r="D59">
+        <v>5.5968999999999998</v>
+      </c>
+      <c r="E59">
+        <v>3.8687999999999998</v>
+      </c>
+      <c r="F59">
+        <v>10.6599</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <v>1.915</v>
+      </c>
+      <c r="D60">
+        <v>5.6451000000000002</v>
+      </c>
+      <c r="E60">
+        <v>3.7930000000000001</v>
+      </c>
+      <c r="F60">
+        <v>10.776300000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>1.9329000000000001</v>
+      </c>
+      <c r="D61">
+        <v>5.5941999999999998</v>
+      </c>
+      <c r="E61" s="2">
+        <v>3.9114</v>
+      </c>
+      <c r="F61" s="1">
+        <v>11.1358</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>128</v>
+      </c>
+      <c r="C62">
+        <v>6.4941000000000004</v>
+      </c>
+      <c r="D62">
+        <v>20.855899999999998</v>
+      </c>
+      <c r="E62">
+        <v>13.496600000000001</v>
+      </c>
+      <c r="F62" s="1">
+        <v>37.027099999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <v>6.4020999999999999</v>
+      </c>
+      <c r="D63">
+        <v>20.7895</v>
+      </c>
+      <c r="E63">
+        <v>13.2775</v>
+      </c>
+      <c r="F63" s="1">
+        <v>37.138500000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <v>6.4958</v>
+      </c>
+      <c r="D64">
+        <v>20.8337</v>
+      </c>
+      <c r="E64">
+        <v>13.4855</v>
+      </c>
+      <c r="F64" s="1">
+        <v>36.439700000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>6.3997999999999999</v>
+      </c>
+      <c r="D65" s="2">
+        <v>21.006900000000002</v>
+      </c>
+      <c r="E65">
+        <v>13.325100000000001</v>
+      </c>
+      <c r="F65" s="1">
+        <v>36.806399999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <v>6.4619</v>
+      </c>
+      <c r="D66">
+        <v>20.902000000000001</v>
+      </c>
+      <c r="E66">
+        <v>14.0307</v>
+      </c>
+      <c r="F66">
+        <v>37.265300000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>512</v>
+      </c>
+      <c r="C67">
+        <v>23.7165</v>
+      </c>
+      <c r="D67">
+        <v>80.766199999999998</v>
+      </c>
+      <c r="E67">
+        <v>50.231699999999996</v>
+      </c>
+      <c r="F67">
+        <v>137.43799999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C68" s="1">
+        <v>23.7712</v>
+      </c>
+      <c r="D68" s="1">
+        <v>80.728800000000007</v>
+      </c>
+      <c r="E68" s="1">
+        <v>49.6922</v>
+      </c>
+      <c r="F68" s="1">
+        <v>137.1865</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C69" s="1">
+        <v>23.7151</v>
+      </c>
+      <c r="D69" s="1">
+        <v>80.937100000000001</v>
+      </c>
+      <c r="E69" s="2">
+        <v>49.585299999999997</v>
+      </c>
+      <c r="F69" s="1">
+        <v>137.4419</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C70" s="1">
+        <v>24.426500000000001</v>
+      </c>
+      <c r="D70" s="1">
+        <v>80.992199999999997</v>
+      </c>
+      <c r="E70" s="1">
+        <v>50.1325</v>
+      </c>
+      <c r="F70" s="1">
+        <v>137.55940000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C71" s="1">
+        <v>23.712399999999999</v>
+      </c>
+      <c r="D71" s="1">
+        <v>80.8035</v>
+      </c>
+      <c r="E71" s="1">
+        <v>49.492800000000003</v>
+      </c>
+      <c r="F71" s="1">
+        <v>137.3143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>1024</v>
+      </c>
+      <c r="C72" s="1">
+        <v>46.428899999999999</v>
+      </c>
+      <c r="D72" s="1">
+        <v>161.9308</v>
+      </c>
+      <c r="E72" s="1">
+        <v>97.304599999999994</v>
+      </c>
+      <c r="F72" s="1">
+        <v>268.89670000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C73" s="1">
+        <v>46.581400000000002</v>
+      </c>
+      <c r="D73" s="1">
+        <v>161.6635</v>
+      </c>
+      <c r="E73" s="2">
+        <v>97.346999999999994</v>
+      </c>
+      <c r="F73" s="1">
+        <v>268.76549999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C74" s="1">
+        <v>46.541600000000003</v>
+      </c>
+      <c r="D74">
+        <v>161.34829999999999</v>
+      </c>
+      <c r="E74">
+        <v>97.814700000000002</v>
+      </c>
+      <c r="F74">
+        <v>267.83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <v>46.716900000000003</v>
+      </c>
+      <c r="D75">
+        <v>161.26140000000001</v>
+      </c>
+      <c r="E75">
+        <v>97.879800000000003</v>
+      </c>
+      <c r="F75">
+        <v>268.09089999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C76" s="1">
+        <v>46.499499999999998</v>
+      </c>
+      <c r="D76" s="1">
+        <v>161.4513</v>
+      </c>
+      <c r="E76" s="1">
+        <v>97.67</v>
+      </c>
+      <c r="F76" s="1">
+        <v>268.19409999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>32</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <v>1.6979</v>
+      </c>
+      <c r="D77">
+        <v>1.7944</v>
+      </c>
+      <c r="E77">
+        <v>1.7821</v>
+      </c>
+      <c r="F77">
+        <v>5.2500999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>1.7670999999999999</v>
+      </c>
+      <c r="D78">
+        <v>1.8374999999999999</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1.7661</v>
+      </c>
+      <c r="F78">
+        <v>4.9379</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C79">
+        <v>1.8048999999999999</v>
+      </c>
+      <c r="D79">
+        <v>1.825</v>
+      </c>
+      <c r="E79">
+        <v>1.6472</v>
+      </c>
+      <c r="F79">
+        <v>4.9217000000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C80">
+        <v>1.7928999999999999</v>
+      </c>
+      <c r="D80">
+        <v>1.9025000000000001</v>
+      </c>
+      <c r="E80">
+        <v>1.6950000000000001</v>
+      </c>
+      <c r="F80">
+        <v>4.0008999999999997</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C81">
+        <v>1.7746999999999999</v>
+      </c>
+      <c r="D81">
+        <v>1.7103999999999999</v>
+      </c>
+      <c r="E81">
+        <v>1.6918</v>
+      </c>
+      <c r="F81">
+        <v>4.8948</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>32</v>
+      </c>
+      <c r="C82">
+        <v>3.7959999999999998</v>
+      </c>
+      <c r="D82">
+        <v>5.4882999999999997</v>
+      </c>
+      <c r="E82">
+        <v>4.1188000000000002</v>
+      </c>
+      <c r="F82">
+        <v>10.8371</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <v>2.8963999999999999</v>
+      </c>
+      <c r="D83">
+        <v>5.5514999999999999</v>
+      </c>
+      <c r="E83">
+        <v>4.1395999999999997</v>
+      </c>
+      <c r="F83">
+        <v>13.6797</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <v>2.8081999999999998</v>
+      </c>
+      <c r="D84">
+        <v>5.7042999999999999</v>
+      </c>
+      <c r="E84">
+        <v>4.7483000000000004</v>
+      </c>
+      <c r="F84">
+        <v>11.081099999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <v>3.2875000000000001</v>
+      </c>
+      <c r="D85">
+        <v>5.5732999999999997</v>
+      </c>
+      <c r="E85">
+        <v>4.1458000000000004</v>
+      </c>
+      <c r="F85">
+        <v>11.100300000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>3.1356999999999999</v>
+      </c>
+      <c r="D86">
+        <v>5.7312000000000003</v>
+      </c>
+      <c r="E86" s="2">
+        <v>4.0510000000000002</v>
+      </c>
+      <c r="F86" s="1">
+        <v>10.538399999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>128</v>
+      </c>
+      <c r="C87">
+        <v>7.4084000000000003</v>
+      </c>
+      <c r="D87">
+        <v>20.8718</v>
+      </c>
+      <c r="E87">
+        <v>13.707800000000001</v>
+      </c>
+      <c r="F87" s="1">
+        <v>35.6997</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <v>7.6940999999999997</v>
+      </c>
+      <c r="D88">
+        <v>20.892399999999999</v>
+      </c>
+      <c r="E88">
+        <v>13.5601</v>
+      </c>
+      <c r="F88" s="1">
+        <v>36.979799999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C89">
+        <v>7.1885000000000003</v>
+      </c>
+      <c r="D89">
+        <v>20.891100000000002</v>
+      </c>
+      <c r="E89">
+        <v>14.0039</v>
+      </c>
+      <c r="F89" s="1">
+        <v>39.548200000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>7.9981</v>
+      </c>
+      <c r="D90" s="2">
+        <v>20.845700000000001</v>
+      </c>
+      <c r="E90">
+        <v>14.650399999999999</v>
+      </c>
+      <c r="F90" s="1">
+        <v>36.4024</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <v>7.1730999999999998</v>
+      </c>
+      <c r="D91">
+        <v>20.8995</v>
+      </c>
+      <c r="E91">
+        <v>13.602499999999999</v>
+      </c>
+      <c r="F91">
+        <v>36.448799999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>512</v>
+      </c>
+      <c r="C92">
+        <v>24.184100000000001</v>
+      </c>
+      <c r="D92">
+        <v>81.042199999999994</v>
+      </c>
+      <c r="E92">
+        <v>49.988300000000002</v>
+      </c>
+      <c r="F92">
+        <v>137.9845</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C93" s="1">
+        <v>24.209499999999998</v>
+      </c>
+      <c r="D93" s="1">
+        <v>81.937200000000004</v>
+      </c>
+      <c r="E93" s="1">
+        <v>49.956499999999998</v>
+      </c>
+      <c r="F93" s="1">
+        <v>137.10130000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C94" s="1">
+        <v>24.339200000000002</v>
+      </c>
+      <c r="D94" s="1">
+        <v>81.511399999999995</v>
+      </c>
+      <c r="E94" s="2">
+        <v>50.128300000000003</v>
+      </c>
+      <c r="F94" s="1">
+        <v>137.50700000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C95" s="1">
+        <v>24.221900000000002</v>
+      </c>
+      <c r="D95" s="1">
+        <v>80.772300000000001</v>
+      </c>
+      <c r="E95" s="1">
+        <v>50.108699999999999</v>
+      </c>
+      <c r="F95" s="1">
+        <v>137.19820000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C96" s="1">
+        <v>24.3489</v>
+      </c>
+      <c r="D96" s="1">
+        <v>80.861099999999993</v>
+      </c>
+      <c r="E96" s="1">
+        <v>49.953800000000001</v>
+      </c>
+      <c r="F96" s="1">
+        <v>136.5967</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>1024</v>
+      </c>
+      <c r="C97" s="1">
+        <v>47.347299999999997</v>
+      </c>
+      <c r="D97" s="1">
+        <v>161.6063</v>
+      </c>
+      <c r="E97" s="1">
+        <v>98.373199999999997</v>
+      </c>
+      <c r="F97" s="1">
+        <v>268.93770000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="C98" s="1">
+        <v>47.456600000000002</v>
+      </c>
+      <c r="D98" s="1">
+        <v>162.35159999999999</v>
+      </c>
+      <c r="E98" s="2">
+        <v>97.899100000000004</v>
+      </c>
+      <c r="F98" s="1">
+        <v>268.49959999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C99" s="1">
+        <v>46.6023</v>
+      </c>
+      <c r="D99">
+        <v>161.85230000000001</v>
+      </c>
+      <c r="E99">
+        <v>97.947199999999995</v>
+      </c>
+      <c r="F99">
+        <v>267.26870000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C100">
+        <v>46.6982</v>
+      </c>
+      <c r="D100">
+        <v>163.41079999999999</v>
+      </c>
+      <c r="E100">
+        <v>97.922200000000004</v>
+      </c>
+      <c r="F100">
+        <v>267.98930000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C101" s="1">
+        <v>47.344900000000003</v>
+      </c>
+      <c r="D101" s="1">
+        <v>161.71</v>
+      </c>
+      <c r="E101" s="1">
+        <v>98.768199999999993</v>
+      </c>
+      <c r="F101" s="1">
+        <v>267.4606</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DA7995-62A2-1746-A6B9-83FD1D34723B}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7502,6 +9705,1746 @@
         <v>1.4425370268391795</v>
       </c>
     </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s">
+        <v>3</v>
+      </c>
+      <c r="I64" t="s">
+        <v>9</v>
+      </c>
+      <c r="J64" t="s">
+        <v>5</v>
+      </c>
+      <c r="K64" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" t="s">
+        <v>1</v>
+      </c>
+      <c r="M64" t="s">
+        <v>2</v>
+      </c>
+      <c r="N64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C2:C6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D65">
+        <f>AVERAGE('Hybrid Lloyd'!D2:D6)</f>
+        <v>0.41176000000000001</v>
+      </c>
+      <c r="E65" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E2:E6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F65" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F2:F6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65">
+        <v>4</v>
+      </c>
+      <c r="J65">
+        <v>8</v>
+      </c>
+      <c r="K65" t="e">
+        <f>B3/C65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L65">
+        <f t="shared" ref="L65:N65" si="34">C3/D65</f>
+        <v>2.8211093841072472</v>
+      </c>
+      <c r="M65" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N65" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>32</v>
+      </c>
+      <c r="C66" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C7:C11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D66">
+        <f>AVERAGE('Hybrid Lloyd'!D7:D11)</f>
+        <v>0.49607999999999997</v>
+      </c>
+      <c r="E66" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E7:E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F66" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F7:F11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J66">
+        <v>32</v>
+      </c>
+      <c r="K66" t="e">
+        <f t="shared" ref="K66:K69" si="35">B4/C66</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L66">
+        <f t="shared" ref="L66:L69" si="36">C4/D66</f>
+        <v>8.515118529269472</v>
+      </c>
+      <c r="M66" t="e">
+        <f t="shared" ref="M66:M69" si="37">D4/E66</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N66" t="e">
+        <f t="shared" ref="N66:N69" si="38">E4/F66</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>128</v>
+      </c>
+      <c r="C67" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C12:C16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D67">
+        <f>AVERAGE('Hybrid Lloyd'!D12:D16)</f>
+        <v>1.2865</v>
+      </c>
+      <c r="E67" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E12:E16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F67" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F12:F16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J67">
+        <v>128</v>
+      </c>
+      <c r="K67" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="36"/>
+        <v>12.753377380489702</v>
+      </c>
+      <c r="M67" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N67" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>512</v>
+      </c>
+      <c r="C68" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C17:C21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D68">
+        <f>AVERAGE('Hybrid Lloyd'!D17:D21)</f>
+        <v>5.0021600000000008</v>
+      </c>
+      <c r="E68" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E17:E21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F68" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F17:F21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J68">
+        <v>512</v>
+      </c>
+      <c r="K68" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="36"/>
+        <v>13.076438978361345</v>
+      </c>
+      <c r="M68" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N68" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>1024</v>
+      </c>
+      <c r="C69" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C22:C26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D69">
+        <f>AVERAGE('Hybrid Lloyd'!D22:D26)</f>
+        <v>8.3778400000000008</v>
+      </c>
+      <c r="E69" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E22:E26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F69" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F22:F26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J69">
+        <v>1024</v>
+      </c>
+      <c r="K69" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="36"/>
+        <v>15.599930292294909</v>
+      </c>
+      <c r="M69" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N69" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>8</v>
+      </c>
+      <c r="B70">
+        <v>8</v>
+      </c>
+      <c r="C70" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C27:C31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D70">
+        <f>AVERAGE('Hybrid Lloyd'!D27:D31)</f>
+        <v>0.42655999999999999</v>
+      </c>
+      <c r="E70" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E27:E31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F70" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F27:F31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70">
+        <v>8</v>
+      </c>
+      <c r="J70">
+        <v>8</v>
+      </c>
+      <c r="K70" t="e">
+        <f>B3/C70</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L70">
+        <f t="shared" ref="L70:N70" si="39">C3/D70</f>
+        <v>2.7232276819204806</v>
+      </c>
+      <c r="M70" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N70" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>32</v>
+      </c>
+      <c r="C71" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C32:C36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D71">
+        <f>AVERAGE('Hybrid Lloyd'!D32:D36)</f>
+        <v>0.68797999999999992</v>
+      </c>
+      <c r="E71" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E32:E36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F71" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F32:F36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J71">
+        <v>32</v>
+      </c>
+      <c r="K71" t="e">
+        <f t="shared" ref="K71:K74" si="40">B4/C71</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L71">
+        <f t="shared" ref="L71:L74" si="41">C4/D71</f>
+        <v>6.1399749992732344</v>
+      </c>
+      <c r="M71" t="e">
+        <f t="shared" ref="M71:M74" si="42">D4/E71</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N71" t="e">
+        <f t="shared" ref="N71:N74" si="43">E4/F71</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>128</v>
+      </c>
+      <c r="C72" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C37:C41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D72">
+        <f>AVERAGE('Hybrid Lloyd'!D37:D41)</f>
+        <v>1.3041400000000001</v>
+      </c>
+      <c r="E72" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E37:E41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F72" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F37:F41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J72">
+        <v>128</v>
+      </c>
+      <c r="K72" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="41"/>
+        <v>12.580873219132917</v>
+      </c>
+      <c r="M72" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N72" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>512</v>
+      </c>
+      <c r="C73" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C42:C46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D73">
+        <f>AVERAGE('Hybrid Lloyd'!D42:D46)</f>
+        <v>3.7204799999999998</v>
+      </c>
+      <c r="E73" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E42:E46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F73" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F42:F46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J73">
+        <v>512</v>
+      </c>
+      <c r="K73" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="41"/>
+        <v>17.581183073151852</v>
+      </c>
+      <c r="M73" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N73" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>1024</v>
+      </c>
+      <c r="C74" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C47:C51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D74">
+        <f>AVERAGE('Hybrid Lloyd'!D47:D51)</f>
+        <v>6.9077399999999995</v>
+      </c>
+      <c r="E74" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E47:E51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F74" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F47:F51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J74">
+        <v>1024</v>
+      </c>
+      <c r="K74" t="e">
+        <f t="shared" si="40"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="41"/>
+        <v>18.919895653281682</v>
+      </c>
+      <c r="M74" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N74" t="e">
+        <f t="shared" si="43"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>16</v>
+      </c>
+      <c r="B75">
+        <v>8</v>
+      </c>
+      <c r="C75" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C52:C56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D75">
+        <f>AVERAGE('Hybrid Lloyd'!D52:D56)</f>
+        <v>0.44394</v>
+      </c>
+      <c r="E75" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E52:E56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F75" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F52:F56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I75">
+        <v>16</v>
+      </c>
+      <c r="J75">
+        <v>8</v>
+      </c>
+      <c r="K75" t="e">
+        <f>B3/C75</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L75">
+        <f t="shared" ref="L75:N75" si="44">C3/D75</f>
+        <v>2.6166148578636754</v>
+      </c>
+      <c r="M75" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N75" t="e">
+        <f t="shared" si="44"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>32</v>
+      </c>
+      <c r="C76" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C57:C61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D76">
+        <f>AVERAGE('Hybrid Lloyd'!D57:D61)</f>
+        <v>0.47942000000000001</v>
+      </c>
+      <c r="E76" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E57:E61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F76" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F57:F61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J76">
+        <v>32</v>
+      </c>
+      <c r="K76" t="e">
+        <f t="shared" ref="K76:K79" si="45">B4/C76</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L76">
+        <f t="shared" ref="L76:L79" si="46">C4/D76</f>
+        <v>8.8110216511618198</v>
+      </c>
+      <c r="M76" t="e">
+        <f t="shared" ref="M76:M79" si="47">D4/E76</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N76" t="e">
+        <f t="shared" ref="N76:N79" si="48">E4/F76</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>128</v>
+      </c>
+      <c r="C77" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C62:C66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D77">
+        <f>AVERAGE('Hybrid Lloyd'!D62:D66)</f>
+        <v>0.51717999999999997</v>
+      </c>
+      <c r="E77" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E62:E66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F77" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F62:F66)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J77">
+        <v>128</v>
+      </c>
+      <c r="K77" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="46"/>
+        <v>31.724389960942037</v>
+      </c>
+      <c r="M77" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N77" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>512</v>
+      </c>
+      <c r="C78" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C67:C71)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D78">
+        <f>AVERAGE('Hybrid Lloyd'!D67:D71)</f>
+        <v>1.1076799999999998</v>
+      </c>
+      <c r="E78" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E67:E71)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F78" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F67:F71)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J78">
+        <v>512</v>
+      </c>
+      <c r="K78" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="46"/>
+        <v>59.051747797197756</v>
+      </c>
+      <c r="M78" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N78" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>1024</v>
+      </c>
+      <c r="C79" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C72:C76)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D79">
+        <f>AVERAGE('Hybrid Lloyd'!D72:D76)</f>
+        <v>2.0264199999999999</v>
+      </c>
+      <c r="E79" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E72:E76)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F79" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F72:F76)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J79">
+        <v>1024</v>
+      </c>
+      <c r="K79" t="e">
+        <f t="shared" si="45"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="46"/>
+        <v>64.494882600842857</v>
+      </c>
+      <c r="M79" t="e">
+        <f t="shared" si="47"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N79" t="e">
+        <f t="shared" si="48"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>32</v>
+      </c>
+      <c r="B80">
+        <v>8</v>
+      </c>
+      <c r="C80" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C77:C81)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D80">
+        <f>AVERAGE('Hybrid Lloyd'!D77:D81)</f>
+        <v>0.54302000000000006</v>
+      </c>
+      <c r="E80" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E77:E81)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F80" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F77:F81)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I80">
+        <v>32</v>
+      </c>
+      <c r="J80">
+        <v>8</v>
+      </c>
+      <c r="K80" t="e">
+        <f>B3/C80</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L80">
+        <f t="shared" ref="L80:N80" si="49">C3/D80</f>
+        <v>2.1391845604213473</v>
+      </c>
+      <c r="M80" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N80" t="e">
+        <f t="shared" si="49"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>32</v>
+      </c>
+      <c r="C81" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C82:C86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D81">
+        <f>AVERAGE('Hybrid Lloyd'!D82:D86)</f>
+        <v>0.50075999999999998</v>
+      </c>
+      <c r="E81" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E82:E86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F81" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F82:F86)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J81">
+        <v>32</v>
+      </c>
+      <c r="K81" t="e">
+        <f t="shared" ref="K81:K84" si="50">B4/C81</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L81">
+        <f t="shared" ref="L81:L84" si="51">C4/D81</f>
+        <v>8.4355379822669541</v>
+      </c>
+      <c r="M81" t="e">
+        <f t="shared" ref="M81:M84" si="52">D4/E81</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N81" t="e">
+        <f t="shared" ref="N81:N84" si="53">E4/F81</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>128</v>
+      </c>
+      <c r="C82" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C87:C91)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D82">
+        <f>AVERAGE('Hybrid Lloyd'!D87:D91)</f>
+        <v>0.50490000000000002</v>
+      </c>
+      <c r="E82" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E87:E91)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F82" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F87:F91)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J82">
+        <v>128</v>
+      </c>
+      <c r="K82" t="e">
+        <f t="shared" si="50"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="51"/>
+        <v>32.49597940186176</v>
+      </c>
+      <c r="M82" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N82" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>512</v>
+      </c>
+      <c r="C83" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C92:C96)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D83">
+        <f>AVERAGE('Hybrid Lloyd'!D92:D96)</f>
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="E83" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E92:E96)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F83" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F92:F96)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J83">
+        <v>512</v>
+      </c>
+      <c r="K83" t="e">
+        <f t="shared" si="50"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="51"/>
+        <v>83.060876190476179</v>
+      </c>
+      <c r="M83" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N83" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>1024</v>
+      </c>
+      <c r="C84" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!C97:C101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D84">
+        <f>AVERAGE('Hybrid Lloyd'!D97:D101)</f>
+        <v>1.2601799999999999</v>
+      </c>
+      <c r="E84" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!E97:E101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F84" t="e">
+        <f>AVERAGE('Hybrid Lloyd'!F97:F101)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J84">
+        <v>1024</v>
+      </c>
+      <c r="K84" t="e">
+        <f t="shared" si="50"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="51"/>
+        <v>103.71035883762637</v>
+      </c>
+      <c r="M84" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N84" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>12</v>
+      </c>
+      <c r="I86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>2</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3</v>
+      </c>
+      <c r="I87" t="s">
+        <v>9</v>
+      </c>
+      <c r="J87" t="s">
+        <v>5</v>
+      </c>
+      <c r="K87" t="s">
+        <v>0</v>
+      </c>
+      <c r="L87" t="s">
+        <v>1</v>
+      </c>
+      <c r="M87" t="s">
+        <v>2</v>
+      </c>
+      <c r="N87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>4</v>
+      </c>
+      <c r="B88">
+        <v>8</v>
+      </c>
+      <c r="C88">
+        <f>AVERAGE('Hybrid YinYang'!C2:C6)</f>
+        <v>0.59763999999999995</v>
+      </c>
+      <c r="D88">
+        <f>AVERAGE('Hybrid YinYang'!D2:D6)</f>
+        <v>2.5175000000000001</v>
+      </c>
+      <c r="E88">
+        <f>AVERAGE('Hybrid YinYang'!E2:E6)</f>
+        <v>1.5619399999999999</v>
+      </c>
+      <c r="F88">
+        <f>AVERAGE('Hybrid YinYang'!F2:F6)</f>
+        <v>5.5609599999999997</v>
+      </c>
+      <c r="I88">
+        <v>4</v>
+      </c>
+      <c r="J88">
+        <v>8</v>
+      </c>
+      <c r="K88">
+        <f>B3/C88</f>
+        <v>37.754065992905431</v>
+      </c>
+      <c r="L88">
+        <f t="shared" ref="L88:N88" si="54">C3/D88</f>
+        <v>0.46141807348560082</v>
+      </c>
+      <c r="M88">
+        <f t="shared" si="54"/>
+        <v>35.747903248524274</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="54"/>
+        <v>9.3917273276556568</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>32</v>
+      </c>
+      <c r="C89">
+        <f>AVERAGE('Hybrid YinYang'!C7:C11)</f>
+        <v>1.80548</v>
+      </c>
+      <c r="D89">
+        <f>AVERAGE('Hybrid YinYang'!D7:D11)</f>
+        <v>8.301400000000001</v>
+      </c>
+      <c r="E89">
+        <f>AVERAGE('Hybrid YinYang'!E7:E11)</f>
+        <v>4.364279999999999</v>
+      </c>
+      <c r="F89">
+        <f>AVERAGE('Hybrid YinYang'!F7:F11)</f>
+        <v>12.278099999999998</v>
+      </c>
+      <c r="J89">
+        <v>32</v>
+      </c>
+      <c r="K89">
+        <f t="shared" ref="K89:K92" si="55">B4/C89</f>
+        <v>39.066497551897562</v>
+      </c>
+      <c r="L89">
+        <f t="shared" ref="L89:L92" si="56">C4/D89</f>
+        <v>0.50885151902088799</v>
+      </c>
+      <c r="M89">
+        <f t="shared" ref="M89:M92" si="57">D4/E89</f>
+        <v>48.242055963412078</v>
+      </c>
+      <c r="N89">
+        <f t="shared" ref="N89:N92" si="58">E4/F89</f>
+        <v>17.305677588551976</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>128</v>
+      </c>
+      <c r="C90">
+        <f>AVERAGE('Hybrid YinYang'!C12:C16)</f>
+        <v>6.1808399999999999</v>
+      </c>
+      <c r="D90">
+        <f>AVERAGE('Hybrid YinYang'!D12:D16)</f>
+        <v>31.77976</v>
+      </c>
+      <c r="E90">
+        <f>AVERAGE('Hybrid YinYang'!E12:E16)</f>
+        <v>14.488579999999999</v>
+      </c>
+      <c r="F90">
+        <f>AVERAGE('Hybrid YinYang'!F12:F16)</f>
+        <v>42.93282</v>
+      </c>
+      <c r="J90">
+        <v>128</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="55"/>
+        <v>24.229447777324765</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="56"/>
+        <v>0.51627891462994069</v>
+      </c>
+      <c r="M90">
+        <f t="shared" si="57"/>
+        <v>17.588604266256599</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="58"/>
+        <v>5.3471530637866316</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>512</v>
+      </c>
+      <c r="C91">
+        <f>AVERAGE('Hybrid YinYang'!C17:C21)</f>
+        <v>23.411719999999999</v>
+      </c>
+      <c r="D91">
+        <f>AVERAGE('Hybrid YinYang'!D17:D21)</f>
+        <v>93.330700000000007</v>
+      </c>
+      <c r="E91">
+        <f>AVERAGE('Hybrid YinYang'!E17:E21)</f>
+        <v>52.317219999999999</v>
+      </c>
+      <c r="F91">
+        <f>AVERAGE('Hybrid YinYang'!F17:F21)</f>
+        <v>141.94765999999998</v>
+      </c>
+      <c r="J91">
+        <v>512</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="55"/>
+        <v>7.7159798596600337</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="56"/>
+        <v>0.70084591672407892</v>
+      </c>
+      <c r="M91">
+        <f t="shared" si="57"/>
+        <v>31.575819204460785</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="58"/>
+        <v>1.4304424602702153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>1024</v>
+      </c>
+      <c r="C92">
+        <f>AVERAGE('Hybrid YinYang'!C22:C26)</f>
+        <v>44.688360000000003</v>
+      </c>
+      <c r="D92">
+        <f>AVERAGE('Hybrid YinYang'!D22:D26)</f>
+        <v>154.9802</v>
+      </c>
+      <c r="E92">
+        <f>AVERAGE('Hybrid YinYang'!E22:E26)</f>
+        <v>102.96010000000001</v>
+      </c>
+      <c r="F92">
+        <f>AVERAGE('Hybrid YinYang'!F22:F26)</f>
+        <v>318.7962</v>
+      </c>
+      <c r="J92">
+        <v>1024</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="55"/>
+        <v>0.81777984244666835</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="56"/>
+        <v>0.84329301420439506</v>
+      </c>
+      <c r="M92">
+        <f t="shared" si="57"/>
+        <v>25.607027706202043</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="58"/>
+        <v>1.266397717413194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>8</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+      <c r="C93">
+        <f>AVERAGE('Hybrid YinYang'!C27:C31)</f>
+        <v>1.5886400000000001</v>
+      </c>
+      <c r="D93">
+        <f>AVERAGE('Hybrid YinYang'!D27:D31)</f>
+        <v>1.6825399999999999</v>
+      </c>
+      <c r="E93">
+        <f>AVERAGE('Hybrid YinYang'!E27:E31)</f>
+        <v>1.4415200000000001</v>
+      </c>
+      <c r="F93">
+        <f>AVERAGE('Hybrid YinYang'!F27:F31)</f>
+        <v>5.8468800000000005</v>
+      </c>
+      <c r="I93">
+        <v>8</v>
+      </c>
+      <c r="J93">
+        <v>8</v>
+      </c>
+      <c r="K93">
+        <f>B3/C93</f>
+        <v>14.202928290865142</v>
+      </c>
+      <c r="L93">
+        <f t="shared" ref="L93:N93" si="59">C3/D93</f>
+        <v>0.69039666218930906</v>
+      </c>
+      <c r="M93">
+        <f t="shared" si="59"/>
+        <v>38.734169487762912</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="59"/>
+        <v>8.9324597050050603</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>32</v>
+      </c>
+      <c r="C94">
+        <f>AVERAGE('Hybrid YinYang'!C32:C36)</f>
+        <v>2.9259399999999998</v>
+      </c>
+      <c r="D94">
+        <f>AVERAGE('Hybrid YinYang'!D32:D36)</f>
+        <v>5.3871000000000002</v>
+      </c>
+      <c r="E94">
+        <f>AVERAGE('Hybrid YinYang'!E32:E36)</f>
+        <v>3.8452399999999995</v>
+      </c>
+      <c r="F94">
+        <f>AVERAGE('Hybrid YinYang'!F32:F36)</f>
+        <v>11.938420000000001</v>
+      </c>
+      <c r="J94">
+        <v>32</v>
+      </c>
+      <c r="K94">
+        <f t="shared" ref="K94:K97" si="60">B4/C94</f>
+        <v>24.106365817480881</v>
+      </c>
+      <c r="L94">
+        <f t="shared" ref="L94:L97" si="61">C4/D94</f>
+        <v>0.78412875201871124</v>
+      </c>
+      <c r="M94">
+        <f t="shared" ref="M94:M97" si="62">D4/E94</f>
+        <v>54.753887923770698</v>
+      </c>
+      <c r="N94">
+        <f t="shared" ref="N94:N97" si="63">E4/F94</f>
+        <v>17.798070431430624</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>128</v>
+      </c>
+      <c r="C95">
+        <f>AVERAGE('Hybrid YinYang'!C37:C41)</f>
+        <v>7.9075199999999999</v>
+      </c>
+      <c r="D95">
+        <f>AVERAGE('Hybrid YinYang'!D37:D41)</f>
+        <v>20.308440000000001</v>
+      </c>
+      <c r="E95">
+        <f>AVERAGE('Hybrid YinYang'!E37:E41)</f>
+        <v>13.638139999999998</v>
+      </c>
+      <c r="F95">
+        <f>AVERAGE('Hybrid YinYang'!F37:F41)</f>
+        <v>43.847079999999991</v>
+      </c>
+      <c r="J95">
+        <v>128</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="60"/>
+        <v>18.938724151187731</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="61"/>
+        <v>0.80790154241290824</v>
+      </c>
+      <c r="M95">
+        <f t="shared" si="62"/>
+        <v>18.685385250481374</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="63"/>
+        <v>5.2356590222199522</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>512</v>
+      </c>
+      <c r="C96">
+        <f>AVERAGE('Hybrid YinYang'!C42:C46)</f>
+        <v>25.886880000000001</v>
+      </c>
+      <c r="D96">
+        <f>AVERAGE('Hybrid YinYang'!D42:D46)</f>
+        <v>77.767139999999998</v>
+      </c>
+      <c r="E96">
+        <f>AVERAGE('Hybrid YinYang'!E42:E46)</f>
+        <v>50.047840000000001</v>
+      </c>
+      <c r="F96">
+        <f>AVERAGE('Hybrid YinYang'!F42:F46)</f>
+        <v>162.49673999999999</v>
+      </c>
+      <c r="J96">
+        <v>512</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="60"/>
+        <v>6.9782206275920462</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="61"/>
+        <v>0.84110641075395076</v>
+      </c>
+      <c r="M96">
+        <f t="shared" si="62"/>
+        <v>33.007599928388515</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="63"/>
+        <v>1.2495509756072645</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>1024</v>
+      </c>
+      <c r="C97">
+        <f>AVERAGE('Hybrid YinYang'!C47:C51)</f>
+        <v>47.821900000000007</v>
+      </c>
+      <c r="D97">
+        <f>AVERAGE('Hybrid YinYang'!D47:D51)</f>
+        <v>155.04740000000001</v>
+      </c>
+      <c r="E97">
+        <f>AVERAGE('Hybrid YinYang'!E47:E51)</f>
+        <v>98.344959999999986</v>
+      </c>
+      <c r="F97">
+        <f>AVERAGE('Hybrid YinYang'!F47:F51)</f>
+        <v>319.40604999999999</v>
+      </c>
+      <c r="J97">
+        <v>1024</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="60"/>
+        <v>0.76419464722229757</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="61"/>
+        <v>0.84292751764944129</v>
+      </c>
+      <c r="M97">
+        <f t="shared" si="62"/>
+        <v>26.808716311779818</v>
+      </c>
+      <c r="N97">
+        <f t="shared" si="63"/>
+        <v>1.263979752418591</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>16</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+      <c r="C98">
+        <f>AVERAGE('Hybrid YinYang'!C52:C56)</f>
+        <v>0.74568000000000001</v>
+      </c>
+      <c r="D98">
+        <f>AVERAGE('Hybrid YinYang'!D52:D56)</f>
+        <v>1.7860400000000003</v>
+      </c>
+      <c r="E98">
+        <f>AVERAGE('Hybrid YinYang'!E52:E56)</f>
+        <v>1.3547799999999999</v>
+      </c>
+      <c r="F98">
+        <f>AVERAGE('Hybrid YinYang'!F52:F56)</f>
+        <v>4.4836800000000006</v>
+      </c>
+      <c r="I98">
+        <v>16</v>
+      </c>
+      <c r="J98">
+        <v>8</v>
+      </c>
+      <c r="K98">
+        <f>B3/C98</f>
+        <v>30.258743697028216</v>
+      </c>
+      <c r="L98">
+        <f t="shared" ref="L98:N98" si="64">C3/D98</f>
+        <v>0.65038856912499154</v>
+      </c>
+      <c r="M98">
+        <f t="shared" si="64"/>
+        <v>41.214130707568756</v>
+      </c>
+      <c r="N98">
+        <f t="shared" si="64"/>
+        <v>11.648248759947183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>32</v>
+      </c>
+      <c r="C99">
+        <f>AVERAGE('Hybrid YinYang'!C57:C61)</f>
+        <v>1.9791000000000001</v>
+      </c>
+      <c r="D99">
+        <f>AVERAGE('Hybrid YinYang'!D57:D61)</f>
+        <v>5.5533999999999999</v>
+      </c>
+      <c r="E99">
+        <f>AVERAGE('Hybrid YinYang'!E57:E61)</f>
+        <v>3.8668199999999997</v>
+      </c>
+      <c r="F99">
+        <f>AVERAGE('Hybrid YinYang'!F57:F61)</f>
+        <v>10.85754</v>
+      </c>
+      <c r="J99">
+        <v>32</v>
+      </c>
+      <c r="K99">
+        <f t="shared" ref="K99:K102" si="65">B4/C99</f>
+        <v>35.639320903440961</v>
+      </c>
+      <c r="L99">
+        <f t="shared" ref="L99:L102" si="66">C4/D99</f>
+        <v>0.76064753124212192</v>
+      </c>
+      <c r="M99">
+        <f t="shared" ref="M99:M102" si="67">D4/E99</f>
+        <v>54.448316704682405</v>
+      </c>
+      <c r="N99">
+        <f t="shared" ref="N99:N102" si="68">E4/F99</f>
+        <v>19.569887838313281</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>128</v>
+      </c>
+      <c r="C100">
+        <f>AVERAGE('Hybrid YinYang'!C62:C66)</f>
+        <v>6.4507399999999988</v>
+      </c>
+      <c r="D100">
+        <f>AVERAGE('Hybrid YinYang'!D62:D66)</f>
+        <v>20.877599999999997</v>
+      </c>
+      <c r="E100">
+        <f>AVERAGE('Hybrid YinYang'!E62:E66)</f>
+        <v>13.523079999999998</v>
+      </c>
+      <c r="F100">
+        <f>AVERAGE('Hybrid YinYang'!F62:F66)</f>
+        <v>36.935400000000001</v>
+      </c>
+      <c r="J100">
+        <v>128</v>
+      </c>
+      <c r="K100">
+        <f t="shared" si="65"/>
+        <v>23.215683782015713</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="66"/>
+        <v>0.78587672912595341</v>
+      </c>
+      <c r="M100">
+        <f t="shared" si="67"/>
+        <v>18.844368294796748</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="68"/>
+        <v>6.2154020262404082</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>512</v>
+      </c>
+      <c r="C101">
+        <f>AVERAGE('Hybrid YinYang'!C67:C71)</f>
+        <v>23.86834</v>
+      </c>
+      <c r="D101">
+        <f>AVERAGE('Hybrid YinYang'!D67:D71)</f>
+        <v>80.845560000000006</v>
+      </c>
+      <c r="E101">
+        <f>AVERAGE('Hybrid YinYang'!E67:E71)</f>
+        <v>49.826900000000002</v>
+      </c>
+      <c r="F101">
+        <f>AVERAGE('Hybrid YinYang'!F67:F71)</f>
+        <v>137.38802000000001</v>
+      </c>
+      <c r="J101">
+        <v>512</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="65"/>
+        <v>7.5683671340361336</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="66"/>
+        <v>0.80907894014216719</v>
+      </c>
+      <c r="M101">
+        <f t="shared" si="67"/>
+        <v>33.153960611637487</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="68"/>
+        <v>1.4779160511957299</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>1024</v>
+      </c>
+      <c r="C102">
+        <f>AVERAGE('Hybrid YinYang'!C72:C76)</f>
+        <v>46.553660000000001</v>
+      </c>
+      <c r="D102">
+        <f>AVERAGE('Hybrid YinYang'!D72:D76)</f>
+        <v>161.53105999999997</v>
+      </c>
+      <c r="E102">
+        <f>AVERAGE('Hybrid YinYang'!E72:E76)</f>
+        <v>97.603219999999993</v>
+      </c>
+      <c r="F102">
+        <f>AVERAGE('Hybrid YinYang'!F72:F76)</f>
+        <v>268.35543999999993</v>
+      </c>
+      <c r="J102">
+        <v>1024</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="65"/>
+        <v>0.785013251374865</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="66"/>
+        <v>0.80909343379533327</v>
+      </c>
+      <c r="M102">
+        <f t="shared" si="67"/>
+        <v>27.012450340606936</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="68"/>
+        <v>1.5044330012464073</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>32</v>
+      </c>
+      <c r="B103">
+        <v>8</v>
+      </c>
+      <c r="C103">
+        <f>AVERAGE('Hybrid YinYang'!C77:C81)</f>
+        <v>1.7674999999999996</v>
+      </c>
+      <c r="D103">
+        <f>AVERAGE('Hybrid YinYang'!D77:D81)</f>
+        <v>1.8139600000000002</v>
+      </c>
+      <c r="E103">
+        <f>AVERAGE('Hybrid YinYang'!E77:E81)</f>
+        <v>1.71644</v>
+      </c>
+      <c r="F103">
+        <f>AVERAGE('Hybrid YinYang'!F77:F81)</f>
+        <v>4.8010799999999998</v>
+      </c>
+      <c r="I103">
+        <v>32</v>
+      </c>
+      <c r="J103">
+        <v>8</v>
+      </c>
+      <c r="K103">
+        <f>B3/C103</f>
+        <v>12.76568033946252</v>
+      </c>
+      <c r="L103">
+        <f t="shared" ref="L103:N103" si="69">C3/D103</f>
+        <v>0.64037795761758798</v>
+      </c>
+      <c r="M103">
+        <f t="shared" si="69"/>
+        <v>32.530167090023532</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="69"/>
+        <v>10.878181575812109</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>32</v>
+      </c>
+      <c r="C104">
+        <f>AVERAGE('Hybrid YinYang'!C82:C86)</f>
+        <v>3.1847599999999998</v>
+      </c>
+      <c r="D104">
+        <f>AVERAGE('Hybrid YinYang'!D82:D86)</f>
+        <v>5.6097200000000003</v>
+      </c>
+      <c r="E104">
+        <f>AVERAGE('Hybrid YinYang'!E82:E86)</f>
+        <v>4.2406999999999995</v>
+      </c>
+      <c r="F104">
+        <f>AVERAGE('Hybrid YinYang'!F82:F86)</f>
+        <v>11.447319999999999</v>
+      </c>
+      <c r="J104">
+        <v>32</v>
+      </c>
+      <c r="K104">
+        <f t="shared" ref="K104:K107" si="70">B4/C104</f>
+        <v>22.147282683781512</v>
+      </c>
+      <c r="L104">
+        <f t="shared" ref="L104:L107" si="71">C4/D104</f>
+        <v>0.75301084546109243</v>
+      </c>
+      <c r="M104">
+        <f t="shared" ref="M104:M107" si="72">D4/E104</f>
+        <v>49.647897752729513</v>
+      </c>
+      <c r="N104">
+        <f t="shared" ref="N104:N107" si="73">E4/F104</f>
+        <v>18.561623157210597</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>128</v>
+      </c>
+      <c r="C105">
+        <f>AVERAGE('Hybrid YinYang'!C87:C91)</f>
+        <v>7.4924400000000002</v>
+      </c>
+      <c r="D105">
+        <f>AVERAGE('Hybrid YinYang'!D87:D91)</f>
+        <v>20.880100000000002</v>
+      </c>
+      <c r="E105">
+        <f>AVERAGE('Hybrid YinYang'!E87:E91)</f>
+        <v>13.90494</v>
+      </c>
+      <c r="F105">
+        <f>AVERAGE('Hybrid YinYang'!F87:F91)</f>
+        <v>37.015779999999999</v>
+      </c>
+      <c r="J105">
+        <v>128</v>
+      </c>
+      <c r="K105">
+        <f t="shared" si="70"/>
+        <v>19.987926496575213</v>
+      </c>
+      <c r="L105">
+        <f t="shared" si="71"/>
+        <v>0.78578263514063629</v>
+      </c>
+      <c r="M105">
+        <f t="shared" si="72"/>
+        <v>18.32686081349506</v>
+      </c>
+      <c r="N105">
+        <f t="shared" si="73"/>
+        <v>6.2019052414943028</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>512</v>
+      </c>
+      <c r="C106">
+        <f>AVERAGE('Hybrid YinYang'!C92:C96)</f>
+        <v>24.260719999999999</v>
+      </c>
+      <c r="D106">
+        <f>AVERAGE('Hybrid YinYang'!D92:D96)</f>
+        <v>81.22484</v>
+      </c>
+      <c r="E106">
+        <f>AVERAGE('Hybrid YinYang'!E92:E96)</f>
+        <v>50.027120000000004</v>
+      </c>
+      <c r="F106">
+        <f>AVERAGE('Hybrid YinYang'!F92:F96)</f>
+        <v>137.27753999999999</v>
+      </c>
+      <c r="J106">
+        <v>512</v>
+      </c>
+      <c r="K106">
+        <f t="shared" si="70"/>
+        <v>7.4459603836984236</v>
+      </c>
+      <c r="L106">
+        <f t="shared" si="71"/>
+        <v>0.80530093995876129</v>
+      </c>
+      <c r="M106">
+        <f t="shared" si="72"/>
+        <v>33.021270862684077</v>
+      </c>
+      <c r="N106">
+        <f t="shared" si="73"/>
+        <v>1.4791054676533395</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>1024</v>
+      </c>
+      <c r="C107">
+        <f>AVERAGE('Hybrid YinYang'!C97:C101)</f>
+        <v>47.089860000000002</v>
+      </c>
+      <c r="D107">
+        <f>AVERAGE('Hybrid YinYang'!D97:D101)</f>
+        <v>162.18620000000001</v>
+      </c>
+      <c r="E107">
+        <f>AVERAGE('Hybrid YinYang'!E97:E101)</f>
+        <v>98.181979999999996</v>
+      </c>
+      <c r="F107">
+        <f>AVERAGE('Hybrid YinYang'!F97:F101)</f>
+        <v>268.03118000000006</v>
+      </c>
+      <c r="J107">
+        <v>1024</v>
+      </c>
+      <c r="K107">
+        <f t="shared" si="70"/>
+        <v>0.77607450945914891</v>
+      </c>
+      <c r="L107">
+        <f t="shared" si="71"/>
+        <v>0.80582515651763209</v>
+      </c>
+      <c r="M107">
+        <f t="shared" si="72"/>
+        <v>26.853218211053939</v>
+      </c>
+      <c r="N107">
+        <f t="shared" si="73"/>
+        <v>1.5062530411573756</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Done testing, lost access to Monsoon....................................
</commit_message>
<xml_diff>
--- a/monsoon/Calculations/Testing Numbers.xlsx
+++ b/monsoon/Calculations/Testing Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinimlay/Documents/School/graduate/CS685 - Graduate Research/kmeans_mpi/monsoon/Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F01EFF-59EE-164F-986E-31C10B7E8CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C0DEAA-AD98-3842-8C40-64CC9F994370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="6" xr2:uid="{BC4CF94B-A0A3-6D4F-B231-01F23389F441}"/>
   </bookViews>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="17">
   <si>
     <t>MSD</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>MPI+OMP Lloyd</t>
+  </si>
+  <si>
+    <t>Speedup (over MPI Yinyang)</t>
+  </si>
+  <si>
+    <t>Speedup (over MPI Lloyd)</t>
+  </si>
+  <si>
+    <t>Speedup (over Seq Yinyang)</t>
   </si>
 </sst>
 </file>
@@ -224,7 +233,1138 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="113">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1527,7 +2667,7 @@
   <dimension ref="A1:G160"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:F101"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7583,10 +8723,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DA7995-62A2-1746-A6B9-83FD1D34723B}">
-  <dimension ref="A1:N107"/>
+  <dimension ref="A1:V107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" topLeftCell="G79" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P98" sqref="P98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7596,6 +8736,8 @@
     <col min="7" max="8" width="11.33203125" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -8589,7 +9731,7 @@
         <v>14.806342326365545</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>1024</v>
       </c>
@@ -8629,7 +9771,7 @@
         <v>19.000203309999751</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -8675,7 +9817,7 @@
         <v>5.622676732008129</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>32</v>
       </c>
@@ -8715,7 +9857,7 @@
         <v>15.07670584361953</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>128</v>
       </c>
@@ -8755,7 +9897,7 @@
         <v>23.038669353543785</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>512</v>
       </c>
@@ -8795,7 +9937,7 @@
         <v>25.31214596298069</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>1024</v>
       </c>
@@ -8835,15 +9977,18 @@
         <v>31.395930346494463</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>11</v>
       </c>
       <c r="I40" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -8880,8 +10025,26 @@
       <c r="N41" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q41" t="s">
+        <v>9</v>
+      </c>
+      <c r="R41" t="s">
+        <v>5</v>
+      </c>
+      <c r="S41" t="s">
+        <v>0</v>
+      </c>
+      <c r="T41" t="s">
+        <v>1</v>
+      </c>
+      <c r="U41" t="s">
+        <v>2</v>
+      </c>
+      <c r="V41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4</v>
       </c>
@@ -8926,8 +10089,30 @@
         <f t="shared" si="14"/>
         <v>8.9103320025932362</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q42">
+        <v>4</v>
+      </c>
+      <c r="R42">
+        <v>8</v>
+      </c>
+      <c r="S42">
+        <f>B11/C42</f>
+        <v>1.6985454545454546</v>
+      </c>
+      <c r="T42">
+        <f t="shared" ref="T42:V42" si="15">C11/D42</f>
+        <v>1.5337576681677956</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="15"/>
+        <v>1.7366453493839933</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="15"/>
+        <v>1.9415736854676355</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>32</v>
       </c>
@@ -8951,7 +10136,7 @@
         <v>32</v>
       </c>
       <c r="K43">
-        <f t="shared" ref="K43:K46" si="15">B4/C43</f>
+        <f t="shared" ref="K43:K46" si="16">B4/C43</f>
         <v>29.491558164622067</v>
       </c>
       <c r="L43">
@@ -8959,15 +10144,34 @@
         <v>0.69795315453451945</v>
       </c>
       <c r="M43">
-        <f t="shared" ref="M43:M46" si="16">D4/E43</f>
+        <f t="shared" ref="M43:M46" si="17">D4/E43</f>
         <v>42.721507069460905</v>
       </c>
       <c r="N43">
-        <f t="shared" ref="N43:N46" si="17">E4/F43</f>
+        <f t="shared" ref="N43:N46" si="18">E4/F43</f>
         <v>14.773814407471429</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R43">
+        <v>32</v>
+      </c>
+      <c r="S43">
+        <f t="shared" ref="S43:S46" si="19">B12/C43</f>
+        <v>1.6223041736701704</v>
+      </c>
+      <c r="T43">
+        <f t="shared" ref="T43:T46" si="20">C12/D43</f>
+        <v>1.4118673416784531</v>
+      </c>
+      <c r="U43">
+        <f t="shared" ref="U43:U46" si="21">D12/E43</f>
+        <v>1.7614807720403229</v>
+      </c>
+      <c r="V43">
+        <f t="shared" ref="V43:V46" si="22">E12/F43</f>
+        <v>1.6622519687448287</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>128</v>
       </c>
@@ -8991,23 +10195,42 @@
         <v>128</v>
       </c>
       <c r="K44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>19.001778898859069</v>
       </c>
       <c r="L44">
-        <f t="shared" ref="L43:L46" si="18">C5/D44</f>
+        <f t="shared" ref="L43:L46" si="23">C5/D44</f>
         <v>0.75002308505998938</v>
       </c>
       <c r="M44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15.551434959954893</v>
       </c>
       <c r="N44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.4166974172226459</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R44">
+        <v>128</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="19"/>
+        <v>1.549207742904706</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="20"/>
+        <v>1.136119570553886</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="21"/>
+        <v>1.5966465118890409</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="22"/>
+        <v>1.5973648537113647</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>512</v>
       </c>
@@ -9031,23 +10254,42 @@
         <v>512</v>
       </c>
       <c r="K45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6.4049198695220539</v>
       </c>
       <c r="L45">
+        <f t="shared" si="23"/>
+        <v>0.79485511885197491</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="17"/>
+        <v>28.71741709291879</v>
+      </c>
+      <c r="N45">
         <f t="shared" si="18"/>
-        <v>0.79485511885197491</v>
-      </c>
-      <c r="M45">
-        <f t="shared" si="16"/>
-        <v>28.71741709291879</v>
-      </c>
-      <c r="N45">
-        <f t="shared" si="17"/>
         <v>1.0892919354248591</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R45">
+        <v>512</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="19"/>
+        <v>1.5040781449439795</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="20"/>
+        <v>1.0248254149720972</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="21"/>
+        <v>1.4359245012224326</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="22"/>
+        <v>1.4233799751313845</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>1024</v>
       </c>
@@ -9071,23 +10313,42 @@
         <v>1024</v>
       </c>
       <c r="K46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.74611418850993738</v>
       </c>
       <c r="L46">
+        <f t="shared" si="23"/>
+        <v>0.79646816734898873</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="17"/>
+        <v>23.271310097642626</v>
+      </c>
+      <c r="N46">
         <f t="shared" si="18"/>
-        <v>0.79646816734898873</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="16"/>
-        <v>23.271310097642626</v>
-      </c>
-      <c r="N46">
-        <f t="shared" si="17"/>
         <v>1.3505621259652447</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R46">
+        <v>1024</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="19"/>
+        <v>1.1349284902888399</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="20"/>
+        <v>1.0039352415279321</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="21"/>
+        <v>1.4445993215886794</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="22"/>
+        <v>1.6563215051685773</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>8</v>
       </c>
@@ -9121,19 +10382,41 @@
         <v>33.641479051736994</v>
       </c>
       <c r="L47">
-        <f t="shared" ref="L47:N47" si="19">C3/D47</f>
+        <f t="shared" ref="L47:N47" si="24">C3/D47</f>
         <v>0.631534881697982</v>
       </c>
       <c r="M47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>39.135427618206535</v>
       </c>
       <c r="N47">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>10.284432069252066</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q47">
+        <v>8</v>
+      </c>
+      <c r="R47">
+        <v>8</v>
+      </c>
+      <c r="S47">
+        <f>B11/C47</f>
+        <v>2.0893096764574328</v>
+      </c>
+      <c r="T47">
+        <f t="shared" ref="T47:V47" si="25">C11/D47</f>
+        <v>1.8812413013221991</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="25"/>
+        <v>2.0708187896883805</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="25"/>
+        <v>2.2409919933205469</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>32</v>
       </c>
@@ -9157,23 +10440,42 @@
         <v>32</v>
       </c>
       <c r="K48">
-        <f t="shared" ref="K48:K51" si="20">B4/C48</f>
+        <f t="shared" ref="K48:K51" si="26">B4/C48</f>
         <v>34.44368590682685</v>
       </c>
       <c r="L48">
-        <f t="shared" ref="L48:L51" si="21">C4/D48</f>
+        <f t="shared" ref="L48:L51" si="27">C4/D48</f>
         <v>0.73963608093627209</v>
       </c>
       <c r="M48">
-        <f t="shared" ref="M48:M51" si="22">D4/E48</f>
+        <f t="shared" ref="M48:M51" si="28">D4/E48</f>
         <v>49.271912868061762</v>
       </c>
       <c r="N48">
-        <f t="shared" ref="N48:N51" si="23">E4/F48</f>
+        <f t="shared" ref="N48:N51" si="29">E4/F48</f>
         <v>15.298035483123128</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R48">
+        <v>32</v>
+      </c>
+      <c r="S48">
+        <f t="shared" ref="S48:S51" si="30">B12/C48</f>
+        <v>1.8947162808868057</v>
+      </c>
+      <c r="T48">
+        <f t="shared" ref="T48:T51" si="31">C12/D48</f>
+        <v>1.4961864139684409</v>
+      </c>
+      <c r="U48">
+        <f t="shared" ref="U48:U51" si="32">D12/E48</f>
+        <v>2.0315652015183501</v>
+      </c>
+      <c r="V48">
+        <f t="shared" ref="V48:V51" si="33">E12/F48</f>
+        <v>1.7212338600171933</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>128</v>
       </c>
@@ -9197,23 +10499,42 @@
         <v>128</v>
       </c>
       <c r="K49">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>21.306448629776433</v>
       </c>
       <c r="L49">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.76894185795832692</v>
       </c>
       <c r="M49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>17.224442206435999</v>
       </c>
       <c r="N49">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>4.8846597565589205</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R49">
+        <v>128</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="30"/>
+        <v>1.7371065817965563</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="31"/>
+        <v>1.1647773393196923</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="32"/>
+        <v>1.7684120879492258</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="33"/>
+        <v>1.7666104512932728</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>512</v>
       </c>
@@ -9237,23 +10558,42 @@
         <v>512</v>
       </c>
       <c r="K50">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>7.0142525986355473</v>
       </c>
       <c r="L50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.80012535743014324</v>
       </c>
       <c r="M50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>30.544400492124637</v>
       </c>
       <c r="N50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1.1659602119042718</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R50">
+        <v>512</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="30"/>
+        <v>1.6471687783209534</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="31"/>
+        <v>1.0316204576280144</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="32"/>
+        <v>1.5272770841430328</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="33"/>
+        <v>1.5235625670699442</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>1024</v>
       </c>
@@ -9277,23 +10617,42 @@
         <v>1024</v>
       </c>
       <c r="K51">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>0.7685272846949569</v>
       </c>
       <c r="L51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>0.80065609169894758</v>
       </c>
       <c r="M51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>24.87267571409317</v>
       </c>
       <c r="N51">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1.427341930182064</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R51">
+        <v>1024</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="30"/>
+        <v>1.1690214774048782</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="31"/>
+        <v>1.0092140524285245</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="32"/>
+        <v>1.5440063456639692</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="33"/>
+        <v>1.7504838087324073</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>16</v>
       </c>
@@ -9327,19 +10686,41 @@
         <v>30.176188947734449</v>
       </c>
       <c r="L52">
-        <f t="shared" ref="L52:N52" si="24">C3/D52</f>
+        <f t="shared" ref="L52:N52" si="34">C3/D52</f>
         <v>0.45426886497309482</v>
       </c>
       <c r="M52">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>34.932482482482477</v>
       </c>
       <c r="N52">
-        <f t="shared" si="24"/>
+        <f t="shared" si="34"/>
         <v>10.909448292572881</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q52">
+        <v>16</v>
+      </c>
+      <c r="R52">
+        <v>8</v>
+      </c>
+      <c r="S52">
+        <f>B11/C52</f>
+        <v>1.874097255657198</v>
+      </c>
+      <c r="T52">
+        <f t="shared" ref="T52:V52" si="35">C11/D52</f>
+        <v>1.3531942184958079</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="35"/>
+        <v>1.8484234234234234</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="35"/>
+        <v>2.3771838941203014</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>32</v>
       </c>
@@ -9363,23 +10744,42 @@
         <v>32</v>
       </c>
       <c r="K53">
-        <f t="shared" ref="K53:K56" si="25">B4/C53</f>
+        <f t="shared" ref="K53:K56" si="36">B4/C53</f>
         <v>36.629888137600105</v>
       </c>
       <c r="L53">
-        <f t="shared" ref="L53:L56" si="26">C4/D53</f>
+        <f t="shared" ref="L53:L56" si="37">C4/D53</f>
         <v>0.54074764393080166</v>
       </c>
       <c r="M53">
-        <f t="shared" ref="M53:M56" si="27">D4/E53</f>
+        <f t="shared" ref="M53:M56" si="38">D4/E53</f>
         <v>50.092275188671167</v>
       </c>
       <c r="N53">
-        <f t="shared" ref="N53:N56" si="28">E4/F53</f>
+        <f t="shared" ref="N53:N56" si="39">E4/F53</f>
         <v>17.413036779649904</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R53">
+        <v>32</v>
+      </c>
+      <c r="S53">
+        <f t="shared" ref="S53:S56" si="40">B12/C53</f>
+        <v>2.01497730553911</v>
+      </c>
+      <c r="T53">
+        <f t="shared" ref="T53:T56" si="41">C12/D53</f>
+        <v>1.0938612908263718</v>
+      </c>
+      <c r="U53">
+        <f t="shared" ref="U53:U56" si="42">D12/E53</f>
+        <v>2.0653901424669532</v>
+      </c>
+      <c r="V53">
+        <f t="shared" ref="V53:V56" si="43">E12/F53</f>
+        <v>1.9591998295417292</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>128</v>
       </c>
@@ -9403,23 +10803,42 @@
         <v>128</v>
       </c>
       <c r="K54">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>22.564161518758475</v>
       </c>
       <c r="L54">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>0.57920823186940518</v>
       </c>
       <c r="M54">
-        <f t="shared" si="27"/>
+        <f t="shared" si="38"/>
         <v>17.901220605301088</v>
       </c>
       <c r="N54">
-        <f t="shared" si="28"/>
+        <f t="shared" si="39"/>
         <v>5.0463634796921815</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R54">
+        <v>128</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="40"/>
+        <v>1.8396474310682536</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="41"/>
+        <v>0.87737273793394133</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="42"/>
+        <v>1.8378960855772446</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="43"/>
+        <v>1.8250930276726551</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>512</v>
       </c>
@@ -9443,23 +10862,42 @@
         <v>512</v>
       </c>
       <c r="K55">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>7.3565563155554186</v>
       </c>
       <c r="L55">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>0.59496532287816828</v>
       </c>
       <c r="M55">
-        <f t="shared" si="27"/>
+        <f t="shared" si="38"/>
         <v>31.610924179358552</v>
       </c>
       <c r="N55">
-        <f t="shared" si="28"/>
+        <f t="shared" si="39"/>
         <v>1.208070863096619</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R55">
+        <v>512</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="40"/>
+        <v>1.7275525379995407</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="41"/>
+        <v>0.76710279578155061</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="42"/>
+        <v>1.580605260861645</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="43"/>
+        <v>1.5785886401525022</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>1024</v>
       </c>
@@ -9483,23 +10921,42 @@
         <v>1024</v>
       </c>
       <c r="K56">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>0.77635148426722211</v>
       </c>
       <c r="L56">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>0.59257328085188099</v>
       </c>
       <c r="M56">
-        <f t="shared" si="27"/>
+        <f t="shared" si="38"/>
         <v>25.729944549973077</v>
       </c>
       <c r="N56">
-        <f t="shared" si="28"/>
+        <f t="shared" si="39"/>
         <v>1.4710329260316597</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R56">
+        <v>1024</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="40"/>
+        <v>1.1809230162645046</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="41"/>
+        <v>0.74692903523708876</v>
+      </c>
+      <c r="U56">
+        <f t="shared" si="42"/>
+        <v>1.5972225149958659</v>
+      </c>
+      <c r="V56">
+        <f t="shared" si="43"/>
+        <v>1.8040661909247084</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>32</v>
       </c>
@@ -9533,19 +10990,41 @@
         <v>28.079222460052765</v>
       </c>
       <c r="L57">
-        <f t="shared" ref="L57:N57" si="29">C3/D57</f>
+        <f t="shared" ref="L57:N57" si="44">C3/D57</f>
         <v>0.56360319447274698</v>
       </c>
       <c r="M57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>36.56299439467756</v>
       </c>
       <c r="N57">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>7.5220821643171112</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q57">
+        <v>32</v>
+      </c>
+      <c r="R57">
+        <v>8</v>
+      </c>
+      <c r="S57">
+        <f>B11/C57</f>
+        <v>1.7438648016327343</v>
+      </c>
+      <c r="T57">
+        <f t="shared" ref="T57:V57" si="45">C11/D57</f>
+        <v>1.6788836812125796</v>
+      </c>
+      <c r="U57">
+        <f t="shared" si="45"/>
+        <v>1.9347006129184348</v>
+      </c>
+      <c r="V57">
+        <f t="shared" si="45"/>
+        <v>1.6390721227798293</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>32</v>
       </c>
@@ -9569,23 +11048,42 @@
         <v>32</v>
       </c>
       <c r="K58">
-        <f t="shared" ref="K58:K61" si="30">B4/C58</f>
+        <f t="shared" ref="K58:K61" si="46">B4/C58</f>
         <v>34.273973002128351</v>
       </c>
       <c r="L58">
-        <f t="shared" ref="L58:L61" si="31">C4/D58</f>
+        <f t="shared" ref="L58:L61" si="47">C4/D58</f>
         <v>0.73852657638284258</v>
       </c>
       <c r="M58">
-        <f t="shared" ref="M58:M61" si="32">D4/E58</f>
+        <f t="shared" ref="M58:M61" si="48">D4/E58</f>
         <v>51.627434344425104</v>
       </c>
       <c r="N58">
-        <f t="shared" ref="N58:N61" si="33">E4/F58</f>
+        <f t="shared" ref="N58:N61" si="49">E4/F58</f>
         <v>16.642764718230207</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R58">
+        <v>32</v>
+      </c>
+      <c r="S58">
+        <f t="shared" ref="S58:S61" si="50">B12/C58</f>
+        <v>1.8853805261572252</v>
+      </c>
+      <c r="T58">
+        <f t="shared" ref="T58:T61" si="51">C12/D58</f>
+        <v>1.4939420323301409</v>
+      </c>
+      <c r="U58">
+        <f t="shared" ref="U58:U61" si="52">D12/E58</f>
+        <v>2.1286873789264611</v>
+      </c>
+      <c r="V58">
+        <f t="shared" ref="V58:V61" si="53">E12/F58</f>
+        <v>1.8725339073059315</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>128</v>
       </c>
@@ -9609,23 +11107,42 @@
         <v>128</v>
       </c>
       <c r="K59">
-        <f t="shared" si="30"/>
+        <f t="shared" si="46"/>
         <v>22.772708333966925</v>
       </c>
       <c r="L59">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>0.77856601896967026</v>
       </c>
       <c r="M59">
-        <f t="shared" si="32"/>
+        <f t="shared" si="48"/>
         <v>18.390503737509761</v>
       </c>
       <c r="N59">
-        <f t="shared" si="33"/>
+        <f t="shared" si="49"/>
         <v>5.2369011521857942</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R59">
+        <v>128</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="50"/>
+        <v>1.8566501728956752</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="51"/>
+        <v>1.179355820826397</v>
+      </c>
+      <c r="U59">
+        <f t="shared" si="52"/>
+        <v>1.8881301770536101</v>
+      </c>
+      <c r="V59">
+        <f t="shared" si="53"/>
+        <v>1.894003834231972</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>512</v>
       </c>
@@ -9649,23 +11166,42 @@
         <v>512</v>
       </c>
       <c r="K60">
-        <f t="shared" si="30"/>
+        <f t="shared" si="46"/>
         <v>7.5017425017607744</v>
       </c>
       <c r="L60">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>0.80445335296509357</v>
       </c>
       <c r="M60">
-        <f t="shared" si="32"/>
+        <f t="shared" si="48"/>
         <v>32.255527117573138</v>
       </c>
       <c r="N60">
-        <f t="shared" si="33"/>
+        <f t="shared" si="49"/>
         <v>1.2578606081924004</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R60">
+        <v>512</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="50"/>
+        <v>1.7616468551912932</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="51"/>
+        <v>1.0372006441486836</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="52"/>
+        <v>1.6128366119454627</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="53"/>
+        <v>1.6436490007697777</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B61">
         <v>1024</v>
       </c>
@@ -9689,31 +11225,53 @@
         <v>1024</v>
       </c>
       <c r="K61">
-        <f t="shared" si="30"/>
+        <f t="shared" si="46"/>
         <v>0.78139444583899775</v>
       </c>
       <c r="L61">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>0.80192102140317756</v>
       </c>
       <c r="M61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="48"/>
         <v>26.185077480884697</v>
       </c>
       <c r="N61">
-        <f t="shared" si="33"/>
+        <f t="shared" si="49"/>
         <v>1.4425370268391795</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R61">
+        <v>1024</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="50"/>
+        <v>1.1885939610761427</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="51"/>
+        <v>1.0108084758596063</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="52"/>
+        <v>1.6254755321431127</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="53"/>
+        <v>1.769118986546466</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>13</v>
       </c>
       <c r="I63" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -9750,8 +11308,26 @@
       <c r="N64" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q64" t="s">
+        <v>9</v>
+      </c>
+      <c r="R64" t="s">
+        <v>5</v>
+      </c>
+      <c r="S64" t="s">
+        <v>0</v>
+      </c>
+      <c r="T64" t="s">
+        <v>1</v>
+      </c>
+      <c r="U64" t="s">
+        <v>2</v>
+      </c>
+      <c r="V64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>4</v>
       </c>
@@ -9785,19 +11361,41 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L65">
-        <f t="shared" ref="L65:N65" si="34">C3/D65</f>
+        <f t="shared" ref="L65:N65" si="54">C3/D65</f>
         <v>2.8211093841072472</v>
       </c>
       <c r="M65" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N65" t="e">
-        <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q65">
+        <v>4</v>
+      </c>
+      <c r="R65">
+        <v>8</v>
+      </c>
+      <c r="S65" t="e">
+        <f>C19/C65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T65">
+        <f t="shared" ref="T65:V80" si="55">D19/D65</f>
+        <v>1.2055080629492907</v>
+      </c>
+      <c r="U65" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V65" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B66">
         <v>32</v>
       </c>
@@ -9821,23 +11419,42 @@
         <v>32</v>
       </c>
       <c r="K66" t="e">
-        <f t="shared" ref="K66:K69" si="35">B4/C66</f>
+        <f t="shared" ref="K66:K69" si="56">B4/C66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L66">
-        <f t="shared" ref="L66:L69" si="36">C4/D66</f>
+        <f t="shared" ref="L66:L69" si="57">C4/D66</f>
         <v>8.515118529269472</v>
       </c>
       <c r="M66" t="e">
-        <f t="shared" ref="M66:M69" si="37">D4/E66</f>
+        <f t="shared" ref="M66:M69" si="58">D4/E66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N66" t="e">
-        <f t="shared" ref="N66:N69" si="38">E4/F66</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" ref="N66:N69" si="59">E4/F66</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R66">
+        <v>32</v>
+      </c>
+      <c r="S66" t="e">
+        <f t="shared" ref="S66:S84" si="60">C20/C66</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="55"/>
+        <v>2.6913804225124975</v>
+      </c>
+      <c r="U66" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V66" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B67">
         <v>128</v>
       </c>
@@ -9861,23 +11478,42 @@
         <v>128</v>
       </c>
       <c r="K67" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L67">
-        <f t="shared" si="36"/>
+        <f t="shared" si="57"/>
         <v>12.753377380489702</v>
       </c>
       <c r="M67" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N67" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R67">
+        <v>128</v>
+      </c>
+      <c r="S67" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T67">
+        <f t="shared" si="55"/>
+        <v>3.3018577535950255</v>
+      </c>
+      <c r="U67" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V67" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B68">
         <v>512</v>
       </c>
@@ -9901,23 +11537,42 @@
         <v>512</v>
       </c>
       <c r="K68" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L68">
-        <f t="shared" si="36"/>
+        <f t="shared" si="57"/>
         <v>13.076438978361345</v>
       </c>
       <c r="M68" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N68" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R68">
+        <v>512</v>
+      </c>
+      <c r="S68" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T68">
+        <f t="shared" si="55"/>
+        <v>3.2928374942025029</v>
+      </c>
+      <c r="U68" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V68" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B69">
         <v>1024</v>
       </c>
@@ -9941,23 +11596,42 @@
         <v>1024</v>
       </c>
       <c r="K69" t="e">
-        <f t="shared" si="35"/>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L69">
-        <f t="shared" si="36"/>
+        <f t="shared" si="57"/>
         <v>15.599930292294909</v>
       </c>
       <c r="M69" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N69" t="e">
-        <f t="shared" si="38"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R69">
+        <v>1024</v>
+      </c>
+      <c r="S69" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T69">
+        <f t="shared" si="55"/>
+        <v>3.9938599925517786</v>
+      </c>
+      <c r="U69" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V69" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>8</v>
       </c>
@@ -9991,19 +11665,41 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L70">
-        <f t="shared" ref="L70:N70" si="39">C3/D70</f>
+        <f t="shared" ref="L70:N70" si="61">C3/D70</f>
         <v>2.7232276819204806</v>
       </c>
       <c r="M70" t="e">
-        <f t="shared" si="39"/>
+        <f t="shared" si="61"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N70" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="61"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q70">
+        <v>8</v>
+      </c>
+      <c r="R70">
+        <v>8</v>
+      </c>
+      <c r="S70" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T70">
+        <f t="shared" si="55"/>
+        <v>1.016972993248312</v>
+      </c>
+      <c r="U70" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V70" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>32</v>
       </c>
@@ -10027,23 +11723,42 @@
         <v>32</v>
       </c>
       <c r="K71" t="e">
-        <f t="shared" ref="K71:K74" si="40">B4/C71</f>
+        <f t="shared" ref="K71:K74" si="62">B4/C71</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L71">
-        <f t="shared" ref="L71:L74" si="41">C4/D71</f>
+        <f t="shared" ref="L71:L74" si="63">C4/D71</f>
         <v>6.1399749992732344</v>
       </c>
       <c r="M71" t="e">
-        <f t="shared" ref="M71:M74" si="42">D4/E71</f>
+        <f t="shared" ref="M71:M74" si="64">D4/E71</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N71" t="e">
-        <f t="shared" ref="N71:N74" si="43">E4/F71</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" ref="N71:N74" si="65">E4/F71</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R71">
+        <v>32</v>
+      </c>
+      <c r="S71" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T71">
+        <f t="shared" si="55"/>
+        <v>0.99235442890781722</v>
+      </c>
+      <c r="U71" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V71" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>128</v>
       </c>
@@ -10067,23 +11782,42 @@
         <v>128</v>
       </c>
       <c r="K72" t="e">
-        <f t="shared" si="40"/>
+        <f t="shared" si="62"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L72">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>12.580873219132917</v>
       </c>
       <c r="M72" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N72" t="e">
-        <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R72">
+        <v>128</v>
+      </c>
+      <c r="S72" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T72">
+        <f t="shared" si="55"/>
+        <v>1.759443004585397</v>
+      </c>
+      <c r="U72" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V72" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>512</v>
       </c>
@@ -10107,23 +11841,42 @@
         <v>512</v>
       </c>
       <c r="K73" t="e">
-        <f t="shared" si="40"/>
+        <f t="shared" si="62"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L73">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>17.581183073151852</v>
       </c>
       <c r="M73" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N73" t="e">
-        <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R73">
+        <v>512</v>
+      </c>
+      <c r="S73" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T73">
+        <f t="shared" si="55"/>
+        <v>3.460634111727519</v>
+      </c>
+      <c r="U73" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V73" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B74">
         <v>1024</v>
       </c>
@@ -10147,23 +11900,42 @@
         <v>1024</v>
       </c>
       <c r="K74" t="e">
-        <f t="shared" si="40"/>
+        <f t="shared" si="62"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L74">
-        <f t="shared" si="41"/>
+        <f t="shared" si="63"/>
         <v>18.919895653281682</v>
       </c>
       <c r="M74" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N74" t="e">
-        <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R74">
+        <v>1024</v>
+      </c>
+      <c r="S74" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T74">
+        <f t="shared" si="55"/>
+        <v>3.6161291536739952</v>
+      </c>
+      <c r="U74" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V74" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>16</v>
       </c>
@@ -10197,19 +11969,41 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L75">
-        <f t="shared" ref="L75:N75" si="44">C3/D75</f>
+        <f t="shared" ref="L75:N75" si="66">C3/D75</f>
         <v>2.6166148578636754</v>
       </c>
       <c r="M75" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="66"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N75" t="e">
-        <f t="shared" si="44"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="66"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q75">
+        <v>16</v>
+      </c>
+      <c r="R75">
+        <v>8</v>
+      </c>
+      <c r="S75" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T75">
+        <f t="shared" si="55"/>
+        <v>0.68928233545073658</v>
+      </c>
+      <c r="U75" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V75" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B76">
         <v>32</v>
       </c>
@@ -10233,23 +12027,42 @@
         <v>32</v>
       </c>
       <c r="K76" t="e">
-        <f t="shared" ref="K76:K79" si="45">B4/C76</f>
+        <f t="shared" ref="K76:K79" si="67">B4/C76</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L76">
-        <f t="shared" ref="L76:L79" si="46">C4/D76</f>
+        <f t="shared" ref="L76:L79" si="68">C4/D76</f>
         <v>8.8110216511618198</v>
       </c>
       <c r="M76" t="e">
-        <f t="shared" ref="M76:M79" si="47">D4/E76</f>
+        <f t="shared" ref="M76:M79" si="69">D4/E76</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N76" t="e">
-        <f t="shared" ref="N76:N79" si="48">E4/F76</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" ref="N76:N79" si="70">E4/F76</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R76">
+        <v>32</v>
+      </c>
+      <c r="S76" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T76">
+        <f t="shared" si="55"/>
+        <v>1.2219348379291644</v>
+      </c>
+      <c r="U76" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V76" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B77">
         <v>128</v>
       </c>
@@ -10273,23 +12086,42 @@
         <v>128</v>
       </c>
       <c r="K77" t="e">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L77">
-        <f t="shared" si="46"/>
+        <f t="shared" si="68"/>
         <v>31.724389960942037</v>
       </c>
       <c r="M77" t="e">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N77" t="e">
-        <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="70"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R77">
+        <v>128</v>
+      </c>
+      <c r="S77" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T77">
+        <f t="shared" si="55"/>
+        <v>2.6842105263157898</v>
+      </c>
+      <c r="U77" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V77" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>512</v>
       </c>
@@ -10313,23 +12145,42 @@
         <v>512</v>
       </c>
       <c r="K78" t="e">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L78">
-        <f t="shared" si="46"/>
+        <f t="shared" si="68"/>
         <v>59.051747797197756</v>
       </c>
       <c r="M78" t="e">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N78" t="e">
-        <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="70"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R78">
+        <v>512</v>
+      </c>
+      <c r="S78" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T78">
+        <f t="shared" si="55"/>
+        <v>4.1768019644662733</v>
+      </c>
+      <c r="U78" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V78" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>1024</v>
       </c>
@@ -10353,23 +12204,42 @@
         <v>1024</v>
       </c>
       <c r="K79" t="e">
-        <f t="shared" si="45"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L79">
-        <f t="shared" si="46"/>
+        <f t="shared" si="68"/>
         <v>64.494882600842857</v>
       </c>
       <c r="M79" t="e">
-        <f t="shared" si="47"/>
+        <f t="shared" si="69"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N79" t="e">
-        <f t="shared" si="48"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="70"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R79">
+        <v>1024</v>
+      </c>
+      <c r="S79" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T79">
+        <f t="shared" si="55"/>
+        <v>4.593174169224544</v>
+      </c>
+      <c r="U79" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V79" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>32</v>
       </c>
@@ -10403,19 +12273,41 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L80">
-        <f t="shared" ref="L80:N80" si="49">C3/D80</f>
+        <f t="shared" ref="L80:N80" si="71">C3/D80</f>
         <v>2.1391845604213473</v>
       </c>
       <c r="M80" t="e">
-        <f t="shared" si="49"/>
+        <f t="shared" si="71"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N80" t="e">
-        <f t="shared" si="49"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="71"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q80">
+        <v>32</v>
+      </c>
+      <c r="R80">
+        <v>8</v>
+      </c>
+      <c r="S80" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T80">
+        <f t="shared" si="55"/>
+        <v>1.1318183492320721</v>
+      </c>
+      <c r="U80" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V80" t="e">
+        <f t="shared" si="55"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B81">
         <v>32</v>
       </c>
@@ -10439,23 +12331,42 @@
         <v>32</v>
       </c>
       <c r="K81" t="e">
-        <f t="shared" ref="K81:K84" si="50">B4/C81</f>
+        <f t="shared" ref="K81:K84" si="72">B4/C81</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L81">
-        <f t="shared" ref="L81:L84" si="51">C4/D81</f>
+        <f t="shared" ref="L81:L84" si="73">C4/D81</f>
         <v>8.4355379822669541</v>
       </c>
       <c r="M81" t="e">
-        <f t="shared" ref="M81:M84" si="52">D4/E81</f>
+        <f t="shared" ref="M81:M84" si="74">D4/E81</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N81" t="e">
-        <f t="shared" ref="N81:N84" si="53">E4/F81</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" ref="N81:N84" si="75">E4/F81</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R81">
+        <v>32</v>
+      </c>
+      <c r="S81" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T81">
+        <f t="shared" ref="T81:T84" si="76">D35/D81</f>
+        <v>1.3810607876028433</v>
+      </c>
+      <c r="U81" t="e">
+        <f t="shared" ref="U81:U84" si="77">E35/E81</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V81" t="e">
+        <f t="shared" ref="V81:V84" si="78">F35/F81</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>128</v>
       </c>
@@ -10479,23 +12390,42 @@
         <v>128</v>
       </c>
       <c r="K82" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="72"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L82">
-        <f t="shared" si="51"/>
+        <f t="shared" si="73"/>
         <v>32.49597940186176</v>
       </c>
       <c r="M82" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N82" t="e">
-        <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="75"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R82">
+        <v>128</v>
+      </c>
+      <c r="S82" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T82">
+        <f t="shared" si="76"/>
+        <v>1.6655179243414537</v>
+      </c>
+      <c r="U82" t="e">
+        <f t="shared" si="77"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V82" t="e">
+        <f t="shared" si="78"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>512</v>
       </c>
@@ -10519,23 +12449,42 @@
         <v>512</v>
       </c>
       <c r="K83" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="72"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L83">
-        <f t="shared" si="51"/>
+        <f t="shared" si="73"/>
         <v>83.060876190476179</v>
       </c>
       <c r="M83" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N83" t="e">
-        <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="75"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R83">
+        <v>512</v>
+      </c>
+      <c r="S83" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T83">
+        <f t="shared" si="76"/>
+        <v>3.7730793650793655</v>
+      </c>
+      <c r="U83" t="e">
+        <f t="shared" si="77"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V83" t="e">
+        <f t="shared" si="78"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B84">
         <v>1024</v>
       </c>
@@ -10559,31 +12508,53 @@
         <v>1024</v>
       </c>
       <c r="K84" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="72"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L84">
-        <f t="shared" si="51"/>
+        <f t="shared" si="73"/>
         <v>103.71035883762637</v>
       </c>
       <c r="M84" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N84" t="e">
-        <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="75"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R84">
+        <v>1024</v>
+      </c>
+      <c r="S84" t="e">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T84">
+        <f t="shared" si="76"/>
+        <v>3.6969163135425096</v>
+      </c>
+      <c r="U84" t="e">
+        <f t="shared" si="77"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V84" t="e">
+        <f t="shared" si="78"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>12</v>
       </c>
       <c r="I86" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -10620,8 +12591,26 @@
       <c r="N87" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q87" t="s">
+        <v>9</v>
+      </c>
+      <c r="R87" t="s">
+        <v>5</v>
+      </c>
+      <c r="S87" t="s">
+        <v>0</v>
+      </c>
+      <c r="T87" t="s">
+        <v>1</v>
+      </c>
+      <c r="U87" t="s">
+        <v>2</v>
+      </c>
+      <c r="V87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>4</v>
       </c>
@@ -10655,19 +12644,41 @@
         <v>37.754065992905431</v>
       </c>
       <c r="L88">
-        <f t="shared" ref="L88:N88" si="54">C3/D88</f>
+        <f t="shared" ref="L88:N88" si="79">C3/D88</f>
         <v>0.46141807348560082</v>
       </c>
       <c r="M88">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>35.747903248524274</v>
       </c>
       <c r="N88">
-        <f t="shared" si="54"/>
+        <f t="shared" si="79"/>
         <v>9.3917273276556568</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q88">
+        <v>4</v>
+      </c>
+      <c r="R88">
+        <v>8</v>
+      </c>
+      <c r="S88">
+        <f>C42/C88</f>
+        <v>1.3804296901144502</v>
+      </c>
+      <c r="T88">
+        <f t="shared" ref="T88:V88" si="80">D42/D88</f>
+        <v>0.89615888778550146</v>
+      </c>
+      <c r="U88">
+        <f t="shared" si="80"/>
+        <v>1.0892095727108595</v>
+      </c>
+      <c r="V88">
+        <f t="shared" si="80"/>
+        <v>1.0540266428818048</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>32</v>
       </c>
@@ -10691,23 +12702,42 @@
         <v>32</v>
       </c>
       <c r="K89">
-        <f t="shared" ref="K89:K92" si="55">B4/C89</f>
+        <f t="shared" ref="K89:K92" si="81">B4/C89</f>
         <v>39.066497551897562</v>
       </c>
       <c r="L89">
-        <f t="shared" ref="L89:L92" si="56">C4/D89</f>
+        <f t="shared" ref="L89:L92" si="82">C4/D89</f>
         <v>0.50885151902088799</v>
       </c>
       <c r="M89">
-        <f t="shared" ref="M89:M92" si="57">D4/E89</f>
+        <f t="shared" ref="M89:M92" si="83">D4/E89</f>
         <v>48.242055963412078</v>
       </c>
       <c r="N89">
-        <f t="shared" ref="N89:N92" si="58">E4/F89</f>
+        <f t="shared" ref="N89:N92" si="84">E4/F89</f>
         <v>17.305677588551976</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R89">
+        <v>32</v>
+      </c>
+      <c r="S89">
+        <f t="shared" ref="S89:S107" si="85">C43/C89</f>
+        <v>1.3246671245319803</v>
+      </c>
+      <c r="T89">
+        <f t="shared" ref="T89:T107" si="86">D43/D89</f>
+        <v>0.72906256775965483</v>
+      </c>
+      <c r="U89">
+        <f t="shared" ref="U89:U107" si="87">E43/E89</f>
+        <v>1.1292217731217979</v>
+      </c>
+      <c r="V89">
+        <f t="shared" ref="V89:V107" si="88">F43/F89</f>
+        <v>1.1713750498855686</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B90">
         <v>128</v>
       </c>
@@ -10731,23 +12761,42 @@
         <v>128</v>
       </c>
       <c r="K90">
-        <f t="shared" si="55"/>
+        <f t="shared" si="81"/>
         <v>24.229447777324765</v>
       </c>
       <c r="L90">
-        <f t="shared" si="56"/>
+        <f t="shared" si="82"/>
         <v>0.51627891462994069</v>
       </c>
       <c r="M90">
-        <f t="shared" si="57"/>
+        <f t="shared" si="83"/>
         <v>17.588604266256599</v>
       </c>
       <c r="N90">
-        <f t="shared" si="58"/>
+        <f t="shared" si="84"/>
         <v>5.3471530637866316</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R90">
+        <v>128</v>
+      </c>
+      <c r="S90">
+        <f t="shared" si="85"/>
+        <v>1.2751147093275348</v>
+      </c>
+      <c r="T90">
+        <f t="shared" si="86"/>
+        <v>0.68835069868369048</v>
+      </c>
+      <c r="U90">
+        <f t="shared" si="87"/>
+        <v>1.1309955841083115</v>
+      </c>
+      <c r="V90">
+        <f t="shared" si="88"/>
+        <v>1.2106677362446725</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B91">
         <v>512</v>
       </c>
@@ -10771,23 +12820,42 @@
         <v>512</v>
       </c>
       <c r="K91">
-        <f t="shared" si="55"/>
+        <f t="shared" si="81"/>
         <v>7.7159798596600337</v>
       </c>
       <c r="L91">
-        <f t="shared" si="56"/>
+        <f t="shared" si="82"/>
         <v>0.70084591672407892</v>
       </c>
       <c r="M91">
-        <f t="shared" si="57"/>
+        <f t="shared" si="83"/>
         <v>31.575819204460785</v>
       </c>
       <c r="N91">
-        <f t="shared" si="58"/>
+        <f t="shared" si="84"/>
         <v>1.4304424602702153</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R91">
+        <v>512</v>
+      </c>
+      <c r="S91">
+        <f t="shared" si="85"/>
+        <v>1.2046957677607626</v>
+      </c>
+      <c r="T91">
+        <f t="shared" si="86"/>
+        <v>0.88172787732225288</v>
+      </c>
+      <c r="U91">
+        <f t="shared" si="87"/>
+        <v>1.0995354875507528</v>
+      </c>
+      <c r="V91">
+        <f t="shared" si="88"/>
+        <v>1.3131855784026309</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B92">
         <v>1024</v>
       </c>
@@ -10811,23 +12879,42 @@
         <v>1024</v>
       </c>
       <c r="K92">
-        <f t="shared" si="55"/>
+        <f t="shared" si="81"/>
         <v>0.81777984244666835</v>
       </c>
       <c r="L92">
-        <f t="shared" si="56"/>
+        <f t="shared" si="82"/>
         <v>0.84329301420439506</v>
       </c>
       <c r="M92">
-        <f t="shared" si="57"/>
+        <f t="shared" si="83"/>
         <v>25.607027706202043</v>
       </c>
       <c r="N92">
-        <f t="shared" si="58"/>
+        <f t="shared" si="84"/>
         <v>1.266397717413194</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R92">
+        <v>1024</v>
+      </c>
+      <c r="S92">
+        <f t="shared" si="85"/>
+        <v>1.096051857799212</v>
+      </c>
+      <c r="T92">
+        <f t="shared" si="86"/>
+        <v>1.0587906068000947</v>
+      </c>
+      <c r="U92">
+        <f t="shared" si="87"/>
+        <v>1.1003689778856081</v>
+      </c>
+      <c r="V92">
+        <f t="shared" si="88"/>
+        <v>0.93768194225652624</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>8</v>
       </c>
@@ -10861,19 +12948,41 @@
         <v>14.202928290865142</v>
       </c>
       <c r="L93">
-        <f t="shared" ref="L93:N93" si="59">C3/D93</f>
+        <f t="shared" ref="L93:N93" si="89">C3/D93</f>
         <v>0.69039666218930906</v>
       </c>
       <c r="M93">
-        <f t="shared" si="59"/>
+        <f t="shared" si="89"/>
         <v>38.734169487762912</v>
       </c>
       <c r="N93">
-        <f t="shared" si="59"/>
+        <f t="shared" si="89"/>
         <v>8.9324597050050603</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q93">
+        <v>8</v>
+      </c>
+      <c r="R93">
+        <v>8</v>
+      </c>
+      <c r="S93">
+        <f t="shared" si="85"/>
+        <v>0.42218501359653537</v>
+      </c>
+      <c r="T93">
+        <f t="shared" si="86"/>
+        <v>1.0932043220369203</v>
+      </c>
+      <c r="U93">
+        <f t="shared" si="87"/>
+        <v>0.98974693379210832</v>
+      </c>
+      <c r="V93">
+        <f t="shared" si="88"/>
+        <v>0.86854185480119306</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B94">
         <v>32</v>
       </c>
@@ -10897,23 +13006,42 @@
         <v>32</v>
       </c>
       <c r="K94">
-        <f t="shared" ref="K94:K97" si="60">B4/C94</f>
+        <f t="shared" ref="K94:K97" si="90">B4/C94</f>
         <v>24.106365817480881</v>
       </c>
       <c r="L94">
-        <f t="shared" ref="L94:L97" si="61">C4/D94</f>
+        <f t="shared" ref="L94:L97" si="91">C4/D94</f>
         <v>0.78412875201871124</v>
       </c>
       <c r="M94">
-        <f t="shared" ref="M94:M97" si="62">D4/E94</f>
+        <f t="shared" ref="M94:M97" si="92">D4/E94</f>
         <v>54.753887923770698</v>
       </c>
       <c r="N94">
-        <f t="shared" ref="N94:N97" si="63">E4/F94</f>
+        <f t="shared" ref="N94:N97" si="93">E4/F94</f>
         <v>17.798070431430624</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R94">
+        <v>32</v>
+      </c>
+      <c r="S94">
+        <f t="shared" si="85"/>
+        <v>0.69987764615815762</v>
+      </c>
+      <c r="T94">
+        <f t="shared" si="86"/>
+        <v>1.0601548142785542</v>
+      </c>
+      <c r="U94">
+        <f t="shared" si="87"/>
+        <v>1.1112596352893449</v>
+      </c>
+      <c r="V94">
+        <f t="shared" si="88"/>
+        <v>1.1634219603599134</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B95">
         <v>128</v>
       </c>
@@ -10937,23 +13065,42 @@
         <v>128</v>
       </c>
       <c r="K95">
-        <f t="shared" si="60"/>
+        <f t="shared" si="90"/>
         <v>18.938724151187731</v>
       </c>
       <c r="L95">
-        <f t="shared" si="61"/>
+        <f t="shared" si="91"/>
         <v>0.80790154241290824</v>
       </c>
       <c r="M95">
-        <f t="shared" si="62"/>
+        <f t="shared" si="92"/>
         <v>18.685385250481374</v>
       </c>
       <c r="N95">
-        <f t="shared" si="63"/>
+        <f t="shared" si="93"/>
         <v>5.2356590222199522</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R95">
+        <v>128</v>
+      </c>
+      <c r="S95">
+        <f t="shared" si="85"/>
+        <v>0.88887287038161145</v>
+      </c>
+      <c r="T95">
+        <f t="shared" si="86"/>
+        <v>1.0506666193956795</v>
+      </c>
+      <c r="U95">
+        <f t="shared" si="87"/>
+        <v>1.084818017706227</v>
+      </c>
+      <c r="V95">
+        <f t="shared" si="88"/>
+        <v>1.0718574646247827</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B96">
         <v>512</v>
       </c>
@@ -10977,23 +13124,42 @@
         <v>512</v>
       </c>
       <c r="K96">
-        <f t="shared" si="60"/>
+        <f t="shared" si="90"/>
         <v>6.9782206275920462</v>
       </c>
       <c r="L96">
-        <f t="shared" si="61"/>
+        <f t="shared" si="91"/>
         <v>0.84110641075395076</v>
       </c>
       <c r="M96">
-        <f t="shared" si="62"/>
+        <f t="shared" si="92"/>
         <v>33.007599928388515</v>
       </c>
       <c r="N96">
-        <f t="shared" si="63"/>
+        <f t="shared" si="93"/>
         <v>1.2495509756072645</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R96">
+        <v>512</v>
+      </c>
+      <c r="S96">
+        <f t="shared" si="85"/>
+        <v>0.99486303486553795</v>
+      </c>
+      <c r="T96">
+        <f t="shared" si="86"/>
+        <v>1.0512182909131029</v>
+      </c>
+      <c r="U96">
+        <f t="shared" si="87"/>
+        <v>1.080643240547444</v>
+      </c>
+      <c r="V96">
+        <f t="shared" si="88"/>
+        <v>1.0716926382646199</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B97">
         <v>1024</v>
       </c>
@@ -11017,23 +13183,42 @@
         <v>1024</v>
       </c>
       <c r="K97">
-        <f t="shared" si="60"/>
+        <f t="shared" si="90"/>
         <v>0.76419464722229757</v>
       </c>
       <c r="L97">
-        <f t="shared" si="61"/>
+        <f t="shared" si="91"/>
         <v>0.84292751764944129</v>
       </c>
       <c r="M97">
-        <f t="shared" si="62"/>
+        <f t="shared" si="92"/>
         <v>26.808716311779818</v>
       </c>
       <c r="N97">
-        <f t="shared" si="63"/>
+        <f t="shared" si="93"/>
         <v>1.263979752418591</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R97">
+        <v>1024</v>
+      </c>
+      <c r="S97">
+        <f t="shared" si="85"/>
+        <v>0.99436241554601545</v>
+      </c>
+      <c r="T97">
+        <f t="shared" si="86"/>
+        <v>1.0527959836798295</v>
+      </c>
+      <c r="U97">
+        <f t="shared" si="87"/>
+        <v>1.0778380508772389</v>
+      </c>
+      <c r="V97">
+        <f t="shared" si="88"/>
+        <v>0.88554797255718853</v>
+      </c>
+    </row>
+    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>16</v>
       </c>
@@ -11067,19 +13252,41 @@
         <v>30.258743697028216</v>
       </c>
       <c r="L98">
-        <f t="shared" ref="L98:N98" si="64">C3/D98</f>
+        <f t="shared" ref="L98:N98" si="94">C3/D98</f>
         <v>0.65038856912499154</v>
       </c>
       <c r="M98">
-        <f t="shared" si="64"/>
+        <f t="shared" si="94"/>
         <v>41.214130707568756</v>
       </c>
       <c r="N98">
-        <f t="shared" si="64"/>
+        <f t="shared" si="94"/>
         <v>11.648248759947183</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q98">
+        <v>16</v>
+      </c>
+      <c r="R98">
+        <v>8</v>
+      </c>
+      <c r="S98">
+        <f t="shared" si="85"/>
+        <v>1.0027357579658833</v>
+      </c>
+      <c r="T98">
+        <f t="shared" si="86"/>
+        <v>1.4317260531679019</v>
+      </c>
+      <c r="U98">
+        <f t="shared" si="87"/>
+        <v>1.1798225542154448</v>
+      </c>
+      <c r="V98">
+        <f t="shared" si="88"/>
+        <v>1.0677211576205257</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B99">
         <v>32</v>
       </c>
@@ -11103,23 +13310,42 @@
         <v>32</v>
       </c>
       <c r="K99">
-        <f t="shared" ref="K99:K102" si="65">B4/C99</f>
+        <f t="shared" ref="K99:K102" si="95">B4/C99</f>
         <v>35.639320903440961</v>
       </c>
       <c r="L99">
-        <f t="shared" ref="L99:L102" si="66">C4/D99</f>
+        <f t="shared" ref="L99:L102" si="96">C4/D99</f>
         <v>0.76064753124212192</v>
       </c>
       <c r="M99">
-        <f t="shared" ref="M99:M102" si="67">D4/E99</f>
+        <f t="shared" ref="M99:M102" si="97">D4/E99</f>
         <v>54.448316704682405</v>
       </c>
       <c r="N99">
-        <f t="shared" ref="N99:N102" si="68">E4/F99</f>
+        <f t="shared" ref="N99:N102" si="98">E4/F99</f>
         <v>19.569887838313281</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R99">
+        <v>32</v>
+      </c>
+      <c r="S99">
+        <f t="shared" si="85"/>
+        <v>0.97295740488100646</v>
+      </c>
+      <c r="T99">
+        <f t="shared" si="86"/>
+        <v>1.4066589836856698</v>
+      </c>
+      <c r="U99">
+        <f t="shared" si="87"/>
+        <v>1.086960344675987</v>
+      </c>
+      <c r="V99">
+        <f t="shared" si="88"/>
+        <v>1.1238641533901788</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B100">
         <v>128</v>
       </c>
@@ -11143,23 +13369,42 @@
         <v>128</v>
       </c>
       <c r="K100">
-        <f t="shared" si="65"/>
+        <f t="shared" si="95"/>
         <v>23.215683782015713</v>
       </c>
       <c r="L100">
-        <f t="shared" si="66"/>
+        <f t="shared" si="96"/>
         <v>0.78587672912595341</v>
       </c>
       <c r="M100">
-        <f t="shared" si="67"/>
+        <f t="shared" si="97"/>
         <v>18.844368294796748</v>
       </c>
       <c r="N100">
-        <f t="shared" si="68"/>
+        <f t="shared" si="98"/>
         <v>6.2154020262404082</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R100">
+        <v>128</v>
+      </c>
+      <c r="S100">
+        <f t="shared" si="85"/>
+        <v>1.0288742066801642</v>
+      </c>
+      <c r="T100">
+        <f t="shared" si="86"/>
+        <v>1.3568120856803465</v>
+      </c>
+      <c r="U100">
+        <f t="shared" si="87"/>
+        <v>1.0526862223694604</v>
+      </c>
+      <c r="V100">
+        <f t="shared" si="88"/>
+        <v>1.2316596002750748</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B101">
         <v>512</v>
       </c>
@@ -11183,23 +13428,42 @@
         <v>512</v>
       </c>
       <c r="K101">
-        <f t="shared" si="65"/>
+        <f t="shared" si="95"/>
         <v>7.5683671340361336</v>
       </c>
       <c r="L101">
-        <f t="shared" si="66"/>
+        <f t="shared" si="96"/>
         <v>0.80907894014216719</v>
       </c>
       <c r="M101">
-        <f t="shared" si="67"/>
+        <f t="shared" si="97"/>
         <v>33.153960611637487</v>
       </c>
       <c r="N101">
-        <f t="shared" si="68"/>
+        <f t="shared" si="98"/>
         <v>1.4779160511957299</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R101">
+        <v>512</v>
+      </c>
+      <c r="S101">
+        <f t="shared" si="85"/>
+        <v>1.0287921154131372</v>
+      </c>
+      <c r="T101">
+        <f t="shared" si="86"/>
+        <v>1.3598757928079166</v>
+      </c>
+      <c r="U101">
+        <f t="shared" si="87"/>
+        <v>1.0488133919629756</v>
+      </c>
+      <c r="V101">
+        <f t="shared" si="88"/>
+        <v>1.2233686750853532</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B102">
         <v>1024</v>
       </c>
@@ -11223,23 +13487,42 @@
         <v>1024</v>
       </c>
       <c r="K102">
-        <f t="shared" si="65"/>
+        <f t="shared" si="95"/>
         <v>0.785013251374865</v>
       </c>
       <c r="L102">
-        <f t="shared" si="66"/>
+        <f t="shared" si="96"/>
         <v>0.80909343379533327</v>
       </c>
       <c r="M102">
-        <f t="shared" si="67"/>
+        <f t="shared" si="97"/>
         <v>27.012450340606936</v>
       </c>
       <c r="N102">
-        <f t="shared" si="68"/>
+        <f t="shared" si="98"/>
         <v>1.5044330012464073</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R102">
+        <v>1024</v>
+      </c>
+      <c r="S102">
+        <f t="shared" si="85"/>
+        <v>1.0111570175148419</v>
+      </c>
+      <c r="T102">
+        <f t="shared" si="86"/>
+        <v>1.3653896656160125</v>
+      </c>
+      <c r="U102">
+        <f t="shared" si="87"/>
+        <v>1.0498448719212339</v>
+      </c>
+      <c r="V102">
+        <f t="shared" si="88"/>
+        <v>1.0227051853318128</v>
+      </c>
+    </row>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>32</v>
       </c>
@@ -11273,19 +13556,41 @@
         <v>12.76568033946252</v>
       </c>
       <c r="L103">
-        <f t="shared" ref="L103:N103" si="69">C3/D103</f>
+        <f t="shared" ref="L103:N103" si="99">C3/D103</f>
         <v>0.64037795761758798</v>
       </c>
       <c r="M103">
-        <f t="shared" si="69"/>
+        <f t="shared" si="99"/>
         <v>32.530167090023532</v>
       </c>
       <c r="N103">
-        <f t="shared" si="69"/>
+        <f t="shared" si="99"/>
         <v>10.878181575812109</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q103">
+        <v>32</v>
+      </c>
+      <c r="R103">
+        <v>8</v>
+      </c>
+      <c r="S103">
+        <f t="shared" si="85"/>
+        <v>0.45463083451202274</v>
+      </c>
+      <c r="T103">
+        <f t="shared" si="86"/>
+        <v>1.1362213058722355</v>
+      </c>
+      <c r="U103">
+        <f t="shared" si="87"/>
+        <v>0.88970194122719115</v>
+      </c>
+      <c r="V103">
+        <f t="shared" si="88"/>
+        <v>1.4461662792538348</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B104">
         <v>32</v>
       </c>
@@ -11309,23 +13614,42 @@
         <v>32</v>
       </c>
       <c r="K104">
-        <f t="shared" ref="K104:K107" si="70">B4/C104</f>
+        <f t="shared" ref="K104:K107" si="100">B4/C104</f>
         <v>22.147282683781512</v>
       </c>
       <c r="L104">
-        <f t="shared" ref="L104:L107" si="71">C4/D104</f>
+        <f t="shared" ref="L104:L107" si="101">C4/D104</f>
         <v>0.75301084546109243</v>
       </c>
       <c r="M104">
-        <f t="shared" ref="M104:M107" si="72">D4/E104</f>
+        <f t="shared" ref="M104:M107" si="102">D4/E104</f>
         <v>49.647897752729513</v>
       </c>
       <c r="N104">
-        <f t="shared" ref="N104:N107" si="73">E4/F104</f>
+        <f t="shared" ref="N104:N107" si="103">E4/F104</f>
         <v>18.561623157210597</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R104">
+        <v>32</v>
+      </c>
+      <c r="S104">
+        <f t="shared" si="85"/>
+        <v>0.64618369987063384</v>
+      </c>
+      <c r="T104">
+        <f t="shared" si="86"/>
+        <v>1.0196123870710123</v>
+      </c>
+      <c r="U104">
+        <f t="shared" si="87"/>
+        <v>0.96165727356332698</v>
+      </c>
+      <c r="V104">
+        <f t="shared" si="88"/>
+        <v>1.1152968555085383</v>
+      </c>
+    </row>
+    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B105">
         <v>128</v>
       </c>
@@ -11349,23 +13673,42 @@
         <v>128</v>
       </c>
       <c r="K105">
-        <f t="shared" si="70"/>
+        <f t="shared" si="100"/>
         <v>19.987926496575213</v>
       </c>
       <c r="L105">
-        <f t="shared" si="71"/>
+        <f t="shared" si="101"/>
         <v>0.78578263514063629</v>
       </c>
       <c r="M105">
-        <f t="shared" si="72"/>
+        <f t="shared" si="102"/>
         <v>18.32686081349506</v>
       </c>
       <c r="N105">
-        <f t="shared" si="73"/>
+        <f t="shared" si="103"/>
         <v>6.2019052414943028</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R105">
+        <v>128</v>
+      </c>
+      <c r="S105">
+        <f t="shared" si="85"/>
+        <v>0.87771406911500138</v>
+      </c>
+      <c r="T105">
+        <f t="shared" si="86"/>
+        <v>1.0092691126958204</v>
+      </c>
+      <c r="U105">
+        <f t="shared" si="87"/>
+        <v>0.99653935939313643</v>
+      </c>
+      <c r="V105">
+        <f t="shared" si="88"/>
+        <v>1.1842700599582126</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B106">
         <v>512</v>
       </c>
@@ -11389,23 +13732,42 @@
         <v>512</v>
       </c>
       <c r="K106">
-        <f t="shared" si="70"/>
+        <f t="shared" si="100"/>
         <v>7.4459603836984236</v>
       </c>
       <c r="L106">
-        <f t="shared" si="71"/>
+        <f t="shared" si="101"/>
         <v>0.80530093995876129</v>
       </c>
       <c r="M106">
-        <f t="shared" si="72"/>
+        <f t="shared" si="102"/>
         <v>33.021270862684077</v>
       </c>
       <c r="N106">
-        <f t="shared" si="73"/>
+        <f t="shared" si="103"/>
         <v>1.4791054676533395</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="R106">
+        <v>512</v>
+      </c>
+      <c r="S106">
+        <f t="shared" si="85"/>
+        <v>0.99256411186477567</v>
+      </c>
+      <c r="T106">
+        <f t="shared" si="86"/>
+        <v>1.0010536185728405</v>
+      </c>
+      <c r="U106">
+        <f t="shared" si="87"/>
+        <v>1.0237399234655122</v>
+      </c>
+      <c r="V106">
+        <f t="shared" si="88"/>
+        <v>1.1758898068831944</v>
+      </c>
+    </row>
+    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B107">
         <v>1024</v>
       </c>
@@ -11429,23 +13791,361 @@
         <v>1024</v>
       </c>
       <c r="K107">
-        <f t="shared" si="70"/>
+        <f t="shared" si="100"/>
         <v>0.77607450945914891</v>
       </c>
       <c r="L107">
-        <f t="shared" si="71"/>
+        <f t="shared" si="101"/>
         <v>0.80582515651763209</v>
       </c>
       <c r="M107">
-        <f t="shared" si="72"/>
+        <f t="shared" si="102"/>
         <v>26.853218211053939</v>
       </c>
       <c r="N107">
-        <f t="shared" si="73"/>
+        <f t="shared" si="103"/>
         <v>1.5062530411573756</v>
       </c>
+      <c r="R107">
+        <v>1024</v>
+      </c>
+      <c r="S107">
+        <f t="shared" si="85"/>
+        <v>0.99319174021753287</v>
+      </c>
+      <c r="T107">
+        <f t="shared" si="86"/>
+        <v>1.0048684783292288</v>
+      </c>
+      <c r="U107">
+        <f t="shared" si="87"/>
+        <v>1.0255160875753371</v>
+      </c>
+      <c r="V107">
+        <f t="shared" si="88"/>
+        <v>1.0441694134242141</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J11:M15">
+    <cfRule type="cellIs" dxfId="87" priority="87" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="86" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="85" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:N23">
+    <cfRule type="cellIs" dxfId="81" priority="82" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="83" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="84" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24:N28">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="80" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="81" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:N33">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="78" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K34:N38">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="74" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K42:N46">
+    <cfRule type="cellIs" dxfId="71" priority="70" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="71" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="72" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47:N51">
+    <cfRule type="cellIs" dxfId="68" priority="67" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="69" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K52:N56">
+    <cfRule type="cellIs" dxfId="65" priority="64" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="66" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K57:N61">
+    <cfRule type="cellIs" dxfId="62" priority="61" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="63" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S42:V46">
+    <cfRule type="cellIs" dxfId="59" priority="58" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="60" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S47:V51">
+    <cfRule type="cellIs" dxfId="56" priority="55" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="57" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S52:V56">
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="54" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S57:V61">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65:N69">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70:N74">
+    <cfRule type="cellIs" dxfId="44" priority="43" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K75:N79">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="42" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80:N84">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S65:V69">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S70:V74">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S75:V79">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S80:V84">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88:N92">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K93:N97">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K98:N102">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K103:N107">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S88:V92">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S93:V97">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S98:V102">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S103:V107">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>